<commit_message>
CIERRE  14 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/BALANCE    ZAVALETA   JULIO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/BALANCE    ZAVALETA   JULIO    2022.xlsx
@@ -794,7 +794,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="1032">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -3891,6 +3891,18 @@
   </si>
   <si>
     <t>BALANCE      ABASTO 4 CARNES    Z A V A L E T A      J U L I O            2 0 2 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>ENCHILADA-QQUESO-CHORIZO</t>
+  </si>
+  <si>
+    <t>POLLO-QUESOS-JAMONES-RES-GELATINA-CHORIZO BLANCO</t>
+  </si>
+  <si>
+    <t>CHORIZO-LONGANIZA-QUESOS-</t>
   </si>
 </sst>
 </file>
@@ -7328,6 +7340,39 @@
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7400,76 +7445,10 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7513,6 +7492,39 @@
     </xf>
     <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7706,6 +7718,15 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="11" fillId="14" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7720,15 +7741,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="18" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7748,7 +7760,7 @@
     <xf numFmtId="49" fontId="11" fillId="23" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7760,8 +7772,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FFFF"/>
       <color rgb="FF00FF99"/>
-      <color rgb="FF66FFFF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFCCFF66"/>
@@ -12552,23 +12564,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
-      <c r="C1" s="711" t="s">
+      <c r="B1" s="685"/>
+      <c r="C1" s="687" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="712"/>
-      <c r="E1" s="712"/>
-      <c r="F1" s="712"/>
-      <c r="G1" s="712"/>
-      <c r="H1" s="712"/>
-      <c r="I1" s="712"/>
-      <c r="J1" s="712"/>
-      <c r="K1" s="712"/>
-      <c r="L1" s="712"/>
-      <c r="M1" s="712"/>
+      <c r="D1" s="688"/>
+      <c r="E1" s="688"/>
+      <c r="F1" s="688"/>
+      <c r="G1" s="688"/>
+      <c r="H1" s="688"/>
+      <c r="I1" s="688"/>
+      <c r="J1" s="688"/>
+      <c r="K1" s="688"/>
+      <c r="L1" s="688"/>
+      <c r="M1" s="688"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -12578,17 +12590,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -12602,14 +12614,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -12619,10 +12631,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="690" t="s">
+      <c r="P4" s="701" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="691"/>
+      <c r="Q4" s="702"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -14063,11 +14075,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="692">
+      <c r="M39" s="703">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="694">
+      <c r="N39" s="705">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -14093,8 +14105,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="693"/>
-      <c r="N40" s="695"/>
+      <c r="M40" s="704"/>
+      <c r="N40" s="706"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -14309,29 +14321,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="696" t="s">
+      <c r="H52" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="697"/>
+      <c r="I52" s="708"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="698">
+      <c r="K52" s="709">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="699"/>
-      <c r="M52" s="700">
+      <c r="L52" s="710"/>
+      <c r="M52" s="711">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="701"/>
+      <c r="N52" s="712"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="702" t="s">
+      <c r="D53" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="702"/>
+      <c r="E53" s="713"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -14342,22 +14354,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="702" t="s">
+      <c r="D54" s="713" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="702"/>
+      <c r="E54" s="713"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="703" t="s">
+      <c r="I54" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="704"/>
-      <c r="K54" s="705">
+      <c r="J54" s="715"/>
+      <c r="K54" s="716">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="706"/>
+      <c r="L54" s="717"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -14390,11 +14402,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="707">
+      <c r="K56" s="718">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="708"/>
+      <c r="L56" s="719"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -14411,22 +14423,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="685" t="s">
+      <c r="D58" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="686"/>
+      <c r="E58" s="697"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="687" t="s">
+      <c r="I58" s="698" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="688"/>
-      <c r="K58" s="689">
+      <c r="J58" s="699"/>
+      <c r="K58" s="700">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="689"/>
+      <c r="L58" s="700"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -14570,12 +14582,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -14590,6 +14596,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17448,7 +17460,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>451</v>
       </c>
@@ -17464,7 +17476,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -17474,21 +17486,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -17506,14 +17518,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -17523,15 +17535,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="750"/>
-      <c r="W4" s="722" t="s">
+      <c r="W4" s="738" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="722"/>
+      <c r="X4" s="738"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17582,8 +17594,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="722"/>
-      <c r="X5" s="722"/>
+      <c r="W5" s="738"/>
+      <c r="X5" s="738"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18346,7 +18358,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="726">
+      <c r="W19" s="742">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -18398,7 +18410,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="727"/>
+      <c r="W20" s="743"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -18447,8 +18459,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -18548,8 +18560,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -18604,8 +18616,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -18653,8 +18665,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -18703,8 +18715,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -18752,9 +18764,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18802,9 +18814,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19136,11 +19148,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="741">
+      <c r="M36" s="730">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="743">
+      <c r="N36" s="732">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -19173,8 +19185,8 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="742"/>
-      <c r="N37" s="744"/>
+      <c r="M37" s="731"/>
+      <c r="N37" s="733"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -19861,26 +19873,26 @@
       <c r="A68" s="98"/>
       <c r="B68" s="99"/>
       <c r="C68" s="1"/>
-      <c r="H68" s="696" t="s">
+      <c r="H68" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="697"/>
+      <c r="I68" s="708"/>
       <c r="J68" s="100"/>
-      <c r="K68" s="698">
+      <c r="K68" s="709">
         <f>I66+L66</f>
         <v>314868.39999999997</v>
       </c>
-      <c r="L68" s="731"/>
+      <c r="L68" s="736"/>
       <c r="M68" s="272"/>
       <c r="N68" s="272"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="13"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D69" s="702" t="s">
+      <c r="D69" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="702"/>
+      <c r="E69" s="713"/>
       <c r="F69" s="312">
         <f>F66-K68-C66</f>
         <v>1594593.8500000003</v>
@@ -19889,22 +19901,22 @@
       <c r="J69" s="103"/>
     </row>
     <row r="70" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D70" s="732" t="s">
+      <c r="D70" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="732"/>
+      <c r="E70" s="737"/>
       <c r="F70" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I70" s="703" t="s">
+      <c r="I70" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="704"/>
-      <c r="K70" s="705">
+      <c r="J70" s="715"/>
+      <c r="K70" s="716">
         <f>F72+F73+F74</f>
         <v>1938640.11</v>
       </c>
-      <c r="L70" s="705"/>
+      <c r="L70" s="716"/>
       <c r="M70" s="404"/>
       <c r="N70" s="404"/>
       <c r="O70" s="404"/>
@@ -19945,11 +19957,11 @@
         <v>15</v>
       </c>
       <c r="J72" s="109"/>
-      <c r="K72" s="707">
+      <c r="K72" s="718">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L72" s="708"/>
+      <c r="L72" s="719"/>
     </row>
     <row r="73" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="110" t="s">
@@ -19966,22 +19978,22 @@
       <c r="C74" s="112">
         <v>44647</v>
       </c>
-      <c r="D74" s="685" t="s">
+      <c r="D74" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="686"/>
+      <c r="E74" s="697"/>
       <c r="F74" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I74" s="687" t="s">
+      <c r="I74" s="698" t="s">
         <v>198</v>
       </c>
-      <c r="J74" s="688"/>
-      <c r="K74" s="689">
+      <c r="J74" s="699"/>
+      <c r="K74" s="700">
         <f>K70+K72</f>
         <v>672071.66000000015</v>
       </c>
-      <c r="L74" s="689"/>
+      <c r="L74" s="700"/>
     </row>
     <row r="75" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C75" s="114"/>
@@ -20128,21 +20140,6 @@
     <sortCondition ref="B34:B42"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M39:N39"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -20158,6 +20155,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22743,7 +22755,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>620</v>
       </c>
@@ -22759,7 +22771,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -22769,21 +22781,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -22801,14 +22813,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -22818,15 +22830,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="750"/>
-      <c r="W4" s="722" t="s">
+      <c r="W4" s="738" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="722"/>
+      <c r="X4" s="738"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22877,8 +22889,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="722"/>
-      <c r="X5" s="722"/>
+      <c r="W5" s="738"/>
+      <c r="X5" s="738"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23637,7 +23649,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="726">
+      <c r="W19" s="742">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -23689,7 +23701,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="727"/>
+      <c r="W20" s="743"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -23738,8 +23750,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -23836,8 +23848,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -23892,8 +23904,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -23939,8 +23951,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -23991,8 +24003,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -24043,9 +24055,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24095,9 +24107,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24701,11 +24713,11 @@
       <c r="L41" s="627">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="741">
+      <c r="M41" s="730">
         <f>SUM(M5:M40)</f>
         <v>2479367.6100000003</v>
       </c>
-      <c r="N41" s="741">
+      <c r="N41" s="730">
         <f>SUM(N5:N40)</f>
         <v>1195667</v>
       </c>
@@ -24743,8 +24755,8 @@
       <c r="L42" s="630">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="742"/>
-      <c r="N42" s="742"/>
+      <c r="M42" s="731"/>
+      <c r="N42" s="731"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="790"/>
     </row>
@@ -25431,26 +25443,26 @@
       <c r="A70" s="98"/>
       <c r="B70" s="99"/>
       <c r="C70" s="1"/>
-      <c r="H70" s="696" t="s">
+      <c r="H70" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="697"/>
+      <c r="I70" s="708"/>
       <c r="J70" s="100"/>
-      <c r="K70" s="698">
+      <c r="K70" s="709">
         <f>I68+L68</f>
         <v>428155.54000000004</v>
       </c>
-      <c r="L70" s="731"/>
+      <c r="L70" s="736"/>
       <c r="M70" s="272"/>
       <c r="N70" s="272"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="13"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D71" s="702" t="s">
+      <c r="D71" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="702"/>
+      <c r="E71" s="713"/>
       <c r="F71" s="312">
         <f>F68-K70-C68</f>
         <v>1631087.67</v>
@@ -25460,22 +25472,22 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D72" s="732" t="s">
+      <c r="D72" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="732"/>
+      <c r="E72" s="737"/>
       <c r="F72" s="111">
         <v>-1884975.46</v>
       </c>
-      <c r="I72" s="703" t="s">
+      <c r="I72" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J72" s="704"/>
-      <c r="K72" s="705">
+      <c r="J72" s="715"/>
+      <c r="K72" s="716">
         <f>F74+F75+F76</f>
         <v>1777829.89</v>
       </c>
-      <c r="L72" s="705"/>
+      <c r="L72" s="716"/>
       <c r="M72" s="404"/>
       <c r="N72" s="404"/>
       <c r="O72" s="404"/>
@@ -25516,11 +25528,11 @@
         <v>15</v>
       </c>
       <c r="J74" s="109"/>
-      <c r="K74" s="707">
+      <c r="K74" s="718">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L74" s="708"/>
+      <c r="L74" s="719"/>
       <c r="P74" s="34"/>
     </row>
     <row r="75" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25539,22 +25551,22 @@
       <c r="C76" s="112">
         <v>44682</v>
       </c>
-      <c r="D76" s="685" t="s">
+      <c r="D76" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="686"/>
+      <c r="E76" s="697"/>
       <c r="F76" s="113">
         <v>2112071.92</v>
       </c>
-      <c r="I76" s="687" t="s">
+      <c r="I76" s="698" t="s">
         <v>854</v>
       </c>
-      <c r="J76" s="688"/>
-      <c r="K76" s="689">
+      <c r="J76" s="699"/>
+      <c r="K76" s="700">
         <f>K72+K74</f>
         <v>-14987.790000000037</v>
       </c>
-      <c r="L76" s="689"/>
+      <c r="L76" s="700"/>
       <c r="P76" s="34"/>
     </row>
     <row r="77" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
@@ -25714,21 +25726,6 @@
     <sortCondition ref="J47:J67"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -25744,6 +25741,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -29040,7 +29052,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>754</v>
       </c>
@@ -29056,7 +29068,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -29066,21 +29078,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -29102,14 +29114,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -29119,15 +29131,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="750"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="817"/>
-      <c r="X4" s="817"/>
+      <c r="W4" s="811"/>
+      <c r="X4" s="811"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29181,8 +29193,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="817"/>
-      <c r="X5" s="817"/>
+      <c r="W5" s="811"/>
+      <c r="X5" s="811"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29948,7 +29960,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="818"/>
+      <c r="W19" s="812"/>
       <c r="X19" s="544"/>
       <c r="Y19" s="233"/>
     </row>
@@ -30002,7 +30014,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="818"/>
+      <c r="W20" s="812"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -30057,8 +30069,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -30169,8 +30181,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -30231,8 +30243,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -30285,8 +30297,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -30341,8 +30353,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -30397,9 +30409,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30453,9 +30465,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31046,11 +31058,11 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="741">
+      <c r="M41" s="730">
         <f>SUM(M5:M40)</f>
         <v>1509924.1</v>
       </c>
-      <c r="N41" s="741">
+      <c r="N41" s="730">
         <f>SUM(N5:N40)</f>
         <v>1012291</v>
       </c>
@@ -31082,8 +31094,8 @@
       <c r="L42" s="640">
         <v>3095.88</v>
       </c>
-      <c r="M42" s="742"/>
-      <c r="N42" s="742"/>
+      <c r="M42" s="731"/>
+      <c r="N42" s="731"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="790"/>
     </row>
@@ -31574,26 +31586,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="696" t="s">
+      <c r="H63" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="697"/>
+      <c r="I63" s="708"/>
       <c r="J63" s="562"/>
-      <c r="K63" s="814">
+      <c r="K63" s="817">
         <f>I61+L61</f>
         <v>340912.75</v>
       </c>
-      <c r="L63" s="815"/>
+      <c r="L63" s="818"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="702" t="s">
+      <c r="D64" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="702"/>
+      <c r="E64" s="713"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>1458827.53</v>
@@ -31602,22 +31614,22 @@
       <c r="J64" s="563"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="732" t="s">
+      <c r="D65" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="732"/>
+      <c r="E65" s="737"/>
       <c r="F65" s="111">
         <v>-1572197.3</v>
       </c>
-      <c r="I65" s="703" t="s">
+      <c r="I65" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="704"/>
-      <c r="K65" s="705">
+      <c r="J65" s="715"/>
+      <c r="K65" s="716">
         <f>F67+F68+F69</f>
         <v>2392765.5300000003</v>
       </c>
-      <c r="L65" s="705"/>
+      <c r="L65" s="716"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="582"/>
@@ -31658,11 +31670,11 @@
         <v>15</v>
       </c>
       <c r="J67" s="109"/>
-      <c r="K67" s="816">
+      <c r="K67" s="813">
         <f>-C4</f>
         <v>-2112071.92</v>
       </c>
-      <c r="L67" s="705"/>
+      <c r="L67" s="716"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -31679,22 +31691,22 @@
       <c r="C69" s="112">
         <v>44710</v>
       </c>
-      <c r="D69" s="685" t="s">
+      <c r="D69" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="686"/>
+      <c r="E69" s="697"/>
       <c r="F69" s="113">
         <v>2546982.16</v>
       </c>
-      <c r="I69" s="811" t="s">
+      <c r="I69" s="814" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="812"/>
-      <c r="K69" s="813">
+      <c r="J69" s="815"/>
+      <c r="K69" s="816">
         <f>K65+K67</f>
         <v>280693.61000000034</v>
       </c>
-      <c r="L69" s="813"/>
+      <c r="L69" s="816"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -31841,6 +31853,21 @@
     <sortCondition ref="J42:J56"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -31856,21 +31883,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K65:L65"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.19" top="0.33" bottom="0.33" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -34228,7 +34240,7 @@
   </sheetPr>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="D19" workbookViewId="0">
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
@@ -34255,7 +34267,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>884</v>
       </c>
@@ -34271,7 +34283,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -34281,21 +34293,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -34313,14 +34325,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -34330,7 +34342,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -36102,11 +36114,11 @@
       <c r="L41" s="39">
         <v>18992.37</v>
       </c>
-      <c r="M41" s="741">
+      <c r="M41" s="730">
         <f>SUM(M5:M40)</f>
         <v>1737024</v>
       </c>
-      <c r="N41" s="741">
+      <c r="N41" s="730">
         <f>SUM(N5:N40)</f>
         <v>1314313</v>
       </c>
@@ -36144,8 +36156,8 @@
       <c r="L42" s="52">
         <v>17035.3</v>
       </c>
-      <c r="M42" s="742"/>
-      <c r="N42" s="742"/>
+      <c r="M42" s="731"/>
+      <c r="N42" s="731"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="790"/>
     </row>
@@ -36828,26 +36840,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="696" t="s">
+      <c r="H69" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="697"/>
+      <c r="I69" s="708"/>
       <c r="J69" s="562"/>
-      <c r="K69" s="814">
+      <c r="K69" s="817">
         <f>I67+L67</f>
         <v>534683.29</v>
       </c>
-      <c r="L69" s="815"/>
+      <c r="L69" s="818"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="702" t="s">
+      <c r="D70" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="702"/>
+      <c r="E70" s="713"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1683028.8699999999</v>
@@ -36856,22 +36868,22 @@
       <c r="J70" s="563"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="732" t="s">
+      <c r="D71" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="732"/>
+      <c r="E71" s="737"/>
       <c r="F71" s="111">
         <v>-2122394.9</v>
       </c>
-      <c r="I71" s="703" t="s">
+      <c r="I71" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="704"/>
-      <c r="K71" s="705">
+      <c r="J71" s="715"/>
+      <c r="K71" s="716">
         <f>F73+F74+F75</f>
         <v>2167293.46</v>
       </c>
-      <c r="L71" s="705"/>
+      <c r="L71" s="716"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="658"/>
@@ -36912,11 +36924,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="816">
+      <c r="K73" s="813">
         <f>-C4</f>
         <v>-2546982.16</v>
       </c>
-      <c r="L73" s="705"/>
+      <c r="L73" s="716"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -36933,22 +36945,22 @@
       <c r="C75" s="112">
         <v>44745</v>
       </c>
-      <c r="D75" s="685" t="s">
+      <c r="D75" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="686"/>
+      <c r="E75" s="697"/>
       <c r="F75" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I75" s="687" t="s">
+      <c r="I75" s="698" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="688"/>
-      <c r="K75" s="689">
+      <c r="J75" s="699"/>
+      <c r="K75" s="700">
         <f>K71+K73</f>
         <v>-379688.70000000019</v>
       </c>
-      <c r="L75" s="689"/>
+      <c r="L75" s="700"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -37095,17 +37107,6 @@
     <sortCondition ref="B42:B51"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
     <mergeCell ref="K73:L73"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="I75:J75"/>
@@ -37117,6 +37118,17 @@
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="K71:L71"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42554,8 +42566,8 @@
   </sheetPr>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -42581,7 +42593,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>1027</v>
       </c>
@@ -42597,7 +42609,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -42607,21 +42619,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -42639,14 +42651,14 @@
       <c r="D4" s="18">
         <v>44745</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -42656,7 +42668,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -42669,29 +42681,40 @@
       <c r="B5" s="24">
         <v>44746</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
+      <c r="C5" s="25">
+        <v>13812</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>1029</v>
+      </c>
       <c r="E5" s="27">
         <v>44746</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="28">
+        <v>120812</v>
+      </c>
       <c r="G5" s="575"/>
       <c r="H5" s="29">
         <v>44746</v>
       </c>
-      <c r="I5" s="30"/>
+      <c r="I5" s="30">
+        <v>4929.5</v>
+      </c>
       <c r="J5" s="37"/>
       <c r="K5" s="31"/>
       <c r="L5" s="9"/>
       <c r="M5" s="32">
-        <v>0</v>
+        <v>62065.5</v>
       </c>
       <c r="N5" s="33">
-        <v>0</v>
+        <v>40005</v>
+      </c>
+      <c r="O5" s="664" t="s">
+        <v>766</v>
       </c>
       <c r="P5" s="34">
         <f>N5+M5+L5+I5+C5</f>
-        <v>0</v>
+        <v>120812</v>
       </c>
       <c r="Q5" s="325">
         <f>P5-F5</f>
@@ -42706,29 +42729,40 @@
       <c r="B6" s="24">
         <v>44747</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="35"/>
+      <c r="C6" s="25">
+        <v>45897</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>1030</v>
+      </c>
       <c r="E6" s="27">
         <v>44747</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="28">
+        <v>96271</v>
+      </c>
       <c r="G6" s="575"/>
       <c r="H6" s="29">
         <v>44747</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="30">
+        <v>1094</v>
+      </c>
       <c r="J6" s="37"/>
       <c r="K6" s="38"/>
       <c r="L6" s="39"/>
       <c r="M6" s="32">
-        <v>0</v>
+        <v>25042</v>
       </c>
       <c r="N6" s="33">
-        <v>0</v>
+        <v>24238</v>
+      </c>
+      <c r="O6" s="664" t="s">
+        <v>766</v>
       </c>
       <c r="P6" s="39">
         <f>N6+M6+L6+I6+C6</f>
-        <v>0</v>
+        <v>96271</v>
       </c>
       <c r="Q6" s="325">
         <f t="shared" ref="Q6:Q40" si="0">P6-F6</f>
@@ -42743,29 +42777,40 @@
       <c r="B7" s="24">
         <v>44748</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="40"/>
+      <c r="C7" s="25">
+        <v>19195</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>1031</v>
+      </c>
       <c r="E7" s="27">
         <v>44748</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="28">
+        <v>85317</v>
+      </c>
       <c r="G7" s="575"/>
       <c r="H7" s="29">
         <v>44748</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="30">
+        <v>4864</v>
+      </c>
       <c r="J7" s="37"/>
       <c r="K7" s="38"/>
       <c r="L7" s="39"/>
       <c r="M7" s="32">
-        <v>0</v>
+        <v>34750</v>
       </c>
       <c r="N7" s="33">
-        <v>0</v>
+        <v>28374</v>
+      </c>
+      <c r="O7" s="664" t="s">
+        <v>766</v>
       </c>
       <c r="P7" s="39">
         <f>N7+M7+L7+I7+C7</f>
-        <v>0</v>
+        <v>87183</v>
       </c>
       <c r="Q7" s="325">
         <v>0</v>
@@ -42799,6 +42844,7 @@
       <c r="N8" s="33">
         <v>0</v>
       </c>
+      <c r="O8" s="664"/>
       <c r="P8" s="39">
         <f t="shared" ref="P8:P40" si="1">N8+M8+L8+I8+C8</f>
         <v>0</v>
@@ -42835,6 +42881,7 @@
       <c r="N9" s="33">
         <v>0</v>
       </c>
+      <c r="O9" s="664"/>
       <c r="P9" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -42872,6 +42919,7 @@
       <c r="N10" s="33">
         <v>0</v>
       </c>
+      <c r="O10" s="664"/>
       <c r="P10" s="39">
         <f>N10+M10+L10+I10+C10</f>
         <v>0</v>
@@ -42909,6 +42957,7 @@
       <c r="N11" s="33">
         <v>0</v>
       </c>
+      <c r="O11" s="664"/>
       <c r="P11" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -42946,6 +42995,7 @@
       <c r="N12" s="33">
         <v>0</v>
       </c>
+      <c r="O12" s="664"/>
       <c r="P12" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -42983,6 +43033,7 @@
       <c r="N13" s="33">
         <v>0</v>
       </c>
+      <c r="O13" s="664"/>
       <c r="P13" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43001,7 +43052,9 @@
         <v>44755</v>
       </c>
       <c r="C14" s="25"/>
-      <c r="D14" s="40"/>
+      <c r="D14" s="40" t="s">
+        <v>1028</v>
+      </c>
       <c r="E14" s="27">
         <v>44755</v>
       </c>
@@ -43058,6 +43111,7 @@
       <c r="N15" s="33">
         <v>0</v>
       </c>
+      <c r="O15" s="664"/>
       <c r="P15" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43095,6 +43149,7 @@
       <c r="N16" s="33">
         <v>0</v>
       </c>
+      <c r="O16" s="664"/>
       <c r="P16" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43132,6 +43187,7 @@
       <c r="N17" s="33">
         <v>0</v>
       </c>
+      <c r="O17" s="664"/>
       <c r="P17" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43169,6 +43225,7 @@
       <c r="N18" s="33">
         <v>0</v>
       </c>
+      <c r="O18" s="664"/>
       <c r="P18" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43206,6 +43263,7 @@
       <c r="N19" s="33">
         <v>0</v>
       </c>
+      <c r="O19" s="664"/>
       <c r="P19" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43243,6 +43301,7 @@
       <c r="N20" s="33">
         <v>0</v>
       </c>
+      <c r="O20" s="664"/>
       <c r="P20" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43280,6 +43339,7 @@
       <c r="N21" s="33">
         <v>0</v>
       </c>
+      <c r="O21" s="664"/>
       <c r="P21" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43317,6 +43377,7 @@
       <c r="N22" s="33">
         <v>0</v>
       </c>
+      <c r="O22" s="664"/>
       <c r="P22" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43354,6 +43415,7 @@
       <c r="N23" s="33">
         <v>0</v>
       </c>
+      <c r="O23" s="664"/>
       <c r="P23" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43391,6 +43453,7 @@
       <c r="N24" s="33">
         <v>0</v>
       </c>
+      <c r="O24" s="664"/>
       <c r="P24" s="39">
         <f>N24+M24+L24+I24+C24</f>
         <v>0</v>
@@ -43428,6 +43491,7 @@
       <c r="N25" s="33">
         <v>0</v>
       </c>
+      <c r="O25" s="664"/>
       <c r="P25" s="283">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -43960,17 +44024,17 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="741">
+      <c r="M41" s="730">
         <f>SUM(M5:M40)</f>
-        <v>0</v>
-      </c>
-      <c r="N41" s="741">
+        <v>121857.5</v>
+      </c>
+      <c r="N41" s="730">
         <f>SUM(N5:N40)</f>
-        <v>0</v>
+        <v>92617</v>
       </c>
       <c r="P41" s="506">
         <f>SUM(P5:P40)</f>
-        <v>0</v>
+        <v>304266</v>
       </c>
       <c r="Q41" s="789">
         <f>SUM(Q5:Q40)</f>
@@ -43990,8 +44054,8 @@
       <c r="J42" s="51"/>
       <c r="K42" s="173"/>
       <c r="L42" s="52"/>
-      <c r="M42" s="742"/>
-      <c r="N42" s="742"/>
+      <c r="M42" s="731"/>
+      <c r="N42" s="731"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="790"/>
     </row>
@@ -44046,7 +44110,7 @@
       <c r="L45" s="39"/>
       <c r="M45" s="791">
         <f>M41+N41</f>
-        <v>0</v>
+        <v>214474.5</v>
       </c>
       <c r="N45" s="792"/>
       <c r="P45" s="34"/>
@@ -44445,7 +44509,7 @@
       </c>
       <c r="C67" s="87">
         <f>SUM(C5:C60)</f>
-        <v>0</v>
+        <v>78904</v>
       </c>
       <c r="D67" s="88"/>
       <c r="E67" s="91" t="s">
@@ -44453,7 +44517,7 @@
       </c>
       <c r="F67" s="90">
         <f>SUM(F5:F60)</f>
-        <v>0</v>
+        <v>302400</v>
       </c>
       <c r="G67" s="576"/>
       <c r="H67" s="91" t="s">
@@ -44461,7 +44525,7 @@
       </c>
       <c r="I67" s="92">
         <f>SUM(I5:I60)</f>
-        <v>0</v>
+        <v>10887.5</v>
       </c>
       <c r="J67" s="93"/>
       <c r="K67" s="94" t="s">
@@ -44487,50 +44551,50 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="696" t="s">
+      <c r="H69" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="697"/>
+      <c r="I69" s="708"/>
       <c r="J69" s="562"/>
-      <c r="K69" s="814">
+      <c r="K69" s="817">
         <f>I67+L67</f>
-        <v>0</v>
-      </c>
-      <c r="L69" s="815"/>
+        <v>10887.5</v>
+      </c>
+      <c r="L69" s="818"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="702" t="s">
+      <c r="D70" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="702"/>
+      <c r="E70" s="713"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
-        <v>0</v>
+        <v>212608.5</v>
       </c>
       <c r="I70" s="102"/>
       <c r="J70" s="563"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="732" t="s">
+      <c r="D71" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="732"/>
+      <c r="E71" s="737"/>
       <c r="F71" s="111">
         <v>0</v>
       </c>
-      <c r="I71" s="703" t="s">
+      <c r="I71" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="704"/>
-      <c r="K71" s="705">
+      <c r="J71" s="715"/>
+      <c r="K71" s="716">
         <f>F73+F74+F75</f>
-        <v>2355426.54</v>
-      </c>
-      <c r="L71" s="705"/>
+        <v>2568035.04</v>
+      </c>
+      <c r="L71" s="716"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="658"/>
@@ -44564,18 +44628,18 @@
       </c>
       <c r="F73" s="96">
         <f>SUM(F70:F72)</f>
-        <v>0</v>
+        <v>212608.5</v>
       </c>
       <c r="H73" s="558"/>
       <c r="I73" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="816">
+      <c r="K73" s="813">
         <f>-C4</f>
         <v>-2355426.54</v>
       </c>
-      <c r="L73" s="705"/>
+      <c r="L73" s="716"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -44590,22 +44654,22 @@
     </row>
     <row r="75" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="112"/>
-      <c r="D75" s="685" t="s">
+      <c r="D75" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="686"/>
+      <c r="E75" s="697"/>
       <c r="F75" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I75" s="687" t="s">
+      <c r="I75" s="698" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="688"/>
-      <c r="K75" s="689">
+      <c r="J75" s="699"/>
+      <c r="K75" s="700">
         <f>K71+K73</f>
-        <v>0</v>
-      </c>
-      <c r="L75" s="689"/>
+        <v>212608.5</v>
+      </c>
+      <c r="L75" s="700"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -44749,16 +44813,9 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="Q41:Q42"/>
     <mergeCell ref="M45:N45"/>
     <mergeCell ref="H69:I69"/>
@@ -44768,9 +44825,16 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K73:L73"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.31496062992125984" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46881,23 +46945,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
-      <c r="C1" s="711" t="s">
+      <c r="B1" s="685"/>
+      <c r="C1" s="687" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="712"/>
-      <c r="E1" s="712"/>
-      <c r="F1" s="712"/>
-      <c r="G1" s="712"/>
-      <c r="H1" s="712"/>
-      <c r="I1" s="712"/>
-      <c r="J1" s="712"/>
-      <c r="K1" s="712"/>
-      <c r="L1" s="712"/>
-      <c r="M1" s="712"/>
+      <c r="D1" s="688"/>
+      <c r="E1" s="688"/>
+      <c r="F1" s="688"/>
+      <c r="G1" s="688"/>
+      <c r="H1" s="688"/>
+      <c r="I1" s="688"/>
+      <c r="J1" s="688"/>
+      <c r="K1" s="688"/>
+      <c r="L1" s="688"/>
+      <c r="M1" s="688"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -46907,21 +46971,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
     </row>
@@ -46936,14 +47000,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -46953,14 +47017,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="722" t="s">
+      <c r="W4" s="738" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="722"/>
+      <c r="X4" s="738"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47011,8 +47075,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="722"/>
-      <c r="X5" s="722"/>
+      <c r="W5" s="738"/>
+      <c r="X5" s="738"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47783,7 +47847,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="726">
+      <c r="W19" s="742">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -47835,7 +47899,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="727"/>
+      <c r="W20" s="743"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -47884,8 +47948,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -47986,8 +48050,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -48041,8 +48105,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -48088,8 +48152,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -48140,8 +48204,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -48189,9 +48253,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48241,9 +48305,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48578,11 +48642,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="741">
+      <c r="M36" s="730">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="743">
+      <c r="N36" s="732">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -48590,7 +48654,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="745">
+      <c r="Q36" s="734">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -48625,13 +48689,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="742"/>
-      <c r="N37" s="744"/>
+      <c r="M37" s="731"/>
+      <c r="N37" s="733"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="746"/>
+      <c r="Q37" s="735"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -48921,26 +48985,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="696" t="s">
+      <c r="H52" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="697"/>
+      <c r="I52" s="708"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="698">
+      <c r="K52" s="709">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="731"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="702" t="s">
+      <c r="D53" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="702"/>
+      <c r="E53" s="713"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -48949,29 +49013,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="732" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="732"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="703" t="s">
+      <c r="I54" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="704"/>
-      <c r="K54" s="705">
+      <c r="J54" s="715"/>
+      <c r="K54" s="716">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="705"/>
-      <c r="M54" s="733" t="s">
+      <c r="L54" s="716"/>
+      <c r="M54" s="722" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="734"/>
-      <c r="O54" s="734"/>
-      <c r="P54" s="734"/>
-      <c r="Q54" s="735"/>
+      <c r="N54" s="723"/>
+      <c r="O54" s="723"/>
+      <c r="P54" s="723"/>
+      <c r="Q54" s="724"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -48985,11 +49049,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="736"/>
-      <c r="N55" s="737"/>
-      <c r="O55" s="737"/>
-      <c r="P55" s="737"/>
-      <c r="Q55" s="738"/>
+      <c r="M55" s="725"/>
+      <c r="N55" s="726"/>
+      <c r="O55" s="726"/>
+      <c r="P55" s="726"/>
+      <c r="Q55" s="727"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -49007,11 +49071,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="707">
+      <c r="K56" s="718">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="708"/>
+      <c r="L56" s="719"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -49028,22 +49092,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="685" t="s">
+      <c r="D58" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="686"/>
+      <c r="E58" s="697"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="687" t="s">
+      <c r="I58" s="698" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="688"/>
-      <c r="K58" s="689">
+      <c r="J58" s="699"/>
+      <c r="K58" s="700">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="689"/>
+      <c r="L58" s="700"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -49187,17 +49251,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -49208,14 +49269,17 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -51958,23 +52022,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
-      <c r="C1" s="711" t="s">
+      <c r="B1" s="685"/>
+      <c r="C1" s="687" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="712"/>
-      <c r="E1" s="712"/>
-      <c r="F1" s="712"/>
-      <c r="G1" s="712"/>
-      <c r="H1" s="712"/>
-      <c r="I1" s="712"/>
-      <c r="J1" s="712"/>
-      <c r="K1" s="712"/>
-      <c r="L1" s="712"/>
-      <c r="M1" s="712"/>
+      <c r="D1" s="688"/>
+      <c r="E1" s="688"/>
+      <c r="F1" s="688"/>
+      <c r="G1" s="688"/>
+      <c r="H1" s="688"/>
+      <c r="I1" s="688"/>
+      <c r="J1" s="688"/>
+      <c r="K1" s="688"/>
+      <c r="L1" s="688"/>
+      <c r="M1" s="688"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -51984,21 +52048,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -52016,14 +52080,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -52033,15 +52097,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="750"/>
-      <c r="W4" s="722" t="s">
+      <c r="W4" s="738" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="722"/>
+      <c r="X4" s="738"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52102,8 +52166,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="722"/>
-      <c r="X5" s="722"/>
+      <c r="W5" s="738"/>
+      <c r="X5" s="738"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52860,7 +52924,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="726">
+      <c r="W19" s="742">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -52912,7 +52976,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="727"/>
+      <c r="W20" s="743"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -52961,8 +53025,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -53063,8 +53127,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -53115,8 +53179,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -53162,8 +53226,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -53211,8 +53275,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -53272,9 +53336,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -53328,9 +53392,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -53646,11 +53710,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="741">
+      <c r="M36" s="730">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="743">
+      <c r="N36" s="732">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -53658,7 +53722,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="745">
+      <c r="Q36" s="734">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -53677,13 +53741,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="742"/>
-      <c r="N37" s="744"/>
+      <c r="M37" s="731"/>
+      <c r="N37" s="733"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="746"/>
+      <c r="Q37" s="735"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -53957,26 +54021,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="696" t="s">
+      <c r="H52" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="697"/>
+      <c r="I52" s="708"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="698">
+      <c r="K52" s="709">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="731"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="702" t="s">
+      <c r="D53" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="702"/>
+      <c r="E53" s="713"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -53985,29 +54049,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="732" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="732"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="703" t="s">
+      <c r="I54" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="704"/>
-      <c r="K54" s="705">
+      <c r="J54" s="715"/>
+      <c r="K54" s="716">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="705"/>
-      <c r="M54" s="733" t="s">
+      <c r="L54" s="716"/>
+      <c r="M54" s="722" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="734"/>
-      <c r="O54" s="734"/>
-      <c r="P54" s="734"/>
-      <c r="Q54" s="735"/>
+      <c r="N54" s="723"/>
+      <c r="O54" s="723"/>
+      <c r="P54" s="723"/>
+      <c r="Q54" s="724"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -54021,11 +54085,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="736"/>
-      <c r="N55" s="737"/>
-      <c r="O55" s="737"/>
-      <c r="P55" s="737"/>
-      <c r="Q55" s="738"/>
+      <c r="M55" s="725"/>
+      <c r="N55" s="726"/>
+      <c r="O55" s="726"/>
+      <c r="P55" s="726"/>
+      <c r="Q55" s="727"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -54043,11 +54107,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="707">
+      <c r="K56" s="718">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="708"/>
+      <c r="L56" s="719"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -54064,22 +54128,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="685" t="s">
+      <c r="D58" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="686"/>
+      <c r="E58" s="697"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="687" t="s">
+      <c r="I58" s="698" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="688"/>
-      <c r="K58" s="689">
+      <c r="J58" s="699"/>
+      <c r="K58" s="700">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="689"/>
+      <c r="L58" s="700"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -54223,13 +54287,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -54239,20 +54310,13 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -56947,7 +57011,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>316</v>
       </c>
@@ -56963,7 +57027,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -56973,21 +57037,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -57005,14 +57069,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -57022,15 +57086,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="750"/>
-      <c r="W4" s="722" t="s">
+      <c r="W4" s="738" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="722"/>
+      <c r="X4" s="738"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57081,8 +57145,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="722"/>
-      <c r="X5" s="722"/>
+      <c r="W5" s="738"/>
+      <c r="X5" s="738"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57846,7 +57910,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="726">
+      <c r="W19" s="742">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -57899,7 +57963,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="727"/>
+      <c r="W20" s="743"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -57948,8 +58012,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -58049,8 +58113,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -58105,8 +58169,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -58151,8 +58215,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -58200,8 +58264,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -58255,9 +58319,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58311,9 +58375,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58624,11 +58688,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="741">
+      <c r="M36" s="730">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="743">
+      <c r="N36" s="732">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -58636,7 +58700,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="745">
+      <c r="Q36" s="734">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -58661,13 +58725,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="742"/>
-      <c r="N37" s="744"/>
+      <c r="M37" s="731"/>
+      <c r="N37" s="733"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="746"/>
+      <c r="Q37" s="735"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -58960,26 +59024,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="696" t="s">
+      <c r="H52" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="697"/>
+      <c r="I52" s="708"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="698">
+      <c r="K52" s="709">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="731"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="702" t="s">
+      <c r="D53" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="702"/>
+      <c r="E53" s="713"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -58988,22 +59052,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="732" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="732"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="703" t="s">
+      <c r="I54" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="704"/>
-      <c r="K54" s="705">
+      <c r="J54" s="715"/>
+      <c r="K54" s="716">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="705"/>
+      <c r="L54" s="716"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -59044,11 +59108,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="707">
+      <c r="K56" s="718">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="708"/>
+      <c r="L56" s="719"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -59065,22 +59129,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="685" t="s">
+      <c r="D58" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="686"/>
+      <c r="E58" s="697"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="687" t="s">
+      <c r="I58" s="698" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="688"/>
-      <c r="K58" s="689">
+      <c r="J58" s="699"/>
+      <c r="K58" s="700">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="689"/>
+      <c r="L58" s="700"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -59224,6 +59288,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -59239,20 +59317,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -62046,7 +62110,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="709"/>
+      <c r="B1" s="685"/>
       <c r="C1" s="751" t="s">
         <v>646</v>
       </c>
@@ -62062,7 +62126,7 @@
       <c r="M1" s="752"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="710"/>
+      <c r="B2" s="686"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -62072,21 +62136,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="713" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="714"/>
+      <c r="B3" s="689" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="690"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="715" t="s">
+      <c r="H3" s="691" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="715"/>
+      <c r="I3" s="691"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="739" t="s">
+      <c r="P3" s="728" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="749" t="s">
@@ -62104,14 +62168,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="716" t="s">
+      <c r="E4" s="692" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="717"/>
-      <c r="H4" s="718" t="s">
+      <c r="F4" s="693"/>
+      <c r="H4" s="694" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="719"/>
+      <c r="I4" s="695"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -62121,15 +62185,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="740"/>
+      <c r="P4" s="729"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="750"/>
-      <c r="W4" s="722" t="s">
+      <c r="W4" s="738" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="722"/>
+      <c r="X4" s="738"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -62180,8 +62244,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="722"/>
-      <c r="X5" s="722"/>
+      <c r="W5" s="738"/>
+      <c r="X5" s="738"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -62942,7 +63006,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="726">
+      <c r="W19" s="742">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -62994,7 +63058,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="727"/>
+      <c r="W20" s="743"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -63043,8 +63107,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="728"/>
-      <c r="X21" s="728"/>
+      <c r="W21" s="744"/>
+      <c r="X21" s="744"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -63143,8 +63207,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="729"/>
-      <c r="X23" s="729"/>
+      <c r="W23" s="745"/>
+      <c r="X23" s="745"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -63199,8 +63263,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="729"/>
-      <c r="X24" s="729"/>
+      <c r="W24" s="745"/>
+      <c r="X24" s="745"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -63248,8 +63312,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="730"/>
-      <c r="X25" s="730"/>
+      <c r="W25" s="746"/>
+      <c r="X25" s="746"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -63297,8 +63361,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="730"/>
-      <c r="X26" s="730"/>
+      <c r="W26" s="746"/>
+      <c r="X26" s="746"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -63346,9 +63410,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="723"/>
-      <c r="X27" s="724"/>
-      <c r="Y27" s="725"/>
+      <c r="W27" s="739"/>
+      <c r="X27" s="740"/>
+      <c r="Y27" s="741"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -63396,9 +63460,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="724"/>
-      <c r="X28" s="724"/>
-      <c r="Y28" s="725"/>
+      <c r="W28" s="740"/>
+      <c r="X28" s="740"/>
+      <c r="Y28" s="741"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -63739,11 +63803,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="741">
+      <c r="M36" s="730">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="743">
+      <c r="N36" s="732">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -63776,8 +63840,8 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="742"/>
-      <c r="N37" s="744"/>
+      <c r="M37" s="731"/>
+      <c r="N37" s="733"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -64084,26 +64148,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="696" t="s">
+      <c r="H52" s="707" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="697"/>
+      <c r="I52" s="708"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="698">
+      <c r="K52" s="709">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="731"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="702" t="s">
+      <c r="D53" s="713" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="702"/>
+      <c r="E53" s="713"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -64112,22 +64176,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="732" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="732"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="703" t="s">
+      <c r="I54" s="714" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="704"/>
-      <c r="K54" s="705">
+      <c r="J54" s="715"/>
+      <c r="K54" s="716">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="705"/>
+      <c r="L54" s="716"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -64168,11 +64232,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="707">
+      <c r="K56" s="718">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="708"/>
+      <c r="L56" s="719"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -64189,22 +64253,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="685" t="s">
+      <c r="D58" s="696" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="686"/>
+      <c r="E58" s="697"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="687" t="s">
+      <c r="I58" s="698" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="688"/>
-      <c r="K58" s="689">
+      <c r="J58" s="699"/>
+      <c r="K58" s="700">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="689"/>
+      <c r="L58" s="700"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -64348,20 +64412,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -64378,6 +64428,20 @@
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cierre 3 ago 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/BALANCE    ZAVALETA   JULIO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/BALANCE    ZAVALETA   JULIO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -794,7 +794,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="1057">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -3945,6 +3945,39 @@
   </si>
   <si>
     <t>Nomina # 29</t>
+  </si>
+  <si>
+    <t>CHORIZO-ENCHILADA-QUESOS-MIXIOTE</t>
+  </si>
+  <si>
+    <t>ABASTOS</t>
+  </si>
+  <si>
+    <t>QUESOS-POLLO-CHORIZO-PATA</t>
+  </si>
+  <si>
+    <t>QUESOS-POLLO-ARABE-SALCHICHA-CHISTORRA</t>
+  </si>
+  <si>
+    <t>LONGANIZA-POLLO-QUESOS-JAMON-CHORIZO</t>
+  </si>
+  <si>
+    <t>PRESTAMO</t>
+  </si>
+  <si>
+    <t>SALCHICHONERIA-QUESOS -POLLO-PASTOR</t>
+  </si>
+  <si>
+    <t>AL PASTOR-QUESOS-POLLO-JAMON-PATA</t>
+  </si>
+  <si>
+    <t>SALSAS-JAMON-QUESO-POLLO</t>
+  </si>
+  <si>
+    <t>NOMINA # 30</t>
+  </si>
+  <si>
+    <t>Nomina #30</t>
   </si>
 </sst>
 </file>
@@ -5984,7 +6017,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="829">
+  <cellXfs count="830">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -7398,6 +7431,7 @@
     </xf>
     <xf numFmtId="165" fontId="73" fillId="14" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="73" fillId="14" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="13" fillId="14" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7827,8 +7861,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FF66FFFF"/>
-      <color rgb="FFFFCCFF"/>
       <color rgb="FF00FF99"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFCCFF66"/>
@@ -12619,23 +12653,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="715" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="716" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="716"/>
-      <c r="E1" s="716"/>
-      <c r="F1" s="716"/>
-      <c r="G1" s="716"/>
-      <c r="H1" s="716"/>
-      <c r="I1" s="716"/>
-      <c r="J1" s="716"/>
-      <c r="K1" s="716"/>
-      <c r="L1" s="716"/>
-      <c r="M1" s="716"/>
+      <c r="D1" s="717"/>
+      <c r="E1" s="717"/>
+      <c r="F1" s="717"/>
+      <c r="G1" s="717"/>
+      <c r="H1" s="717"/>
+      <c r="I1" s="717"/>
+      <c r="J1" s="717"/>
+      <c r="K1" s="717"/>
+      <c r="L1" s="717"/>
+      <c r="M1" s="717"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -12645,17 +12679,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -12669,14 +12703,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -12686,10 +12720,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="694" t="s">
+      <c r="P4" s="695" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="695"/>
+      <c r="Q4" s="696"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -14130,11 +14164,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="696">
+      <c r="M39" s="697">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="698">
+      <c r="N39" s="699">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -14160,8 +14194,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="697"/>
-      <c r="N40" s="699"/>
+      <c r="M40" s="698"/>
+      <c r="N40" s="700"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -14376,29 +14410,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="700" t="s">
+      <c r="H52" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="701"/>
+      <c r="I52" s="702"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="702">
+      <c r="K52" s="703">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="703"/>
-      <c r="M52" s="704">
+      <c r="L52" s="704"/>
+      <c r="M52" s="705">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="705"/>
+      <c r="N52" s="706"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="706" t="s">
+      <c r="D53" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="706"/>
+      <c r="E53" s="707"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -14409,22 +14443,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="706" t="s">
+      <c r="D54" s="707" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="706"/>
+      <c r="E54" s="707"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="707" t="s">
+      <c r="I54" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="708"/>
-      <c r="K54" s="709">
+      <c r="J54" s="709"/>
+      <c r="K54" s="710">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="710"/>
+      <c r="L54" s="711"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -14457,11 +14491,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="711">
+      <c r="K56" s="712">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="712"/>
+      <c r="L56" s="713"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -14478,22 +14512,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="689" t="s">
+      <c r="D58" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="690"/>
+      <c r="E58" s="691"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="691" t="s">
+      <c r="I58" s="692" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="692"/>
-      <c r="K58" s="693">
+      <c r="J58" s="693"/>
+      <c r="K58" s="694">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="693"/>
+      <c r="L58" s="694"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -17117,10 +17151,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I76" s="785" t="s">
+      <c r="I76" s="786" t="s">
         <v>597</v>
       </c>
-      <c r="J76" s="786"/>
+      <c r="J76" s="787"/>
       <c r="K76" s="69"/>
       <c r="L76" s="148"/>
       <c r="M76" s="69"/>
@@ -17139,8 +17173,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I77" s="787"/>
-      <c r="J77" s="788"/>
+      <c r="I77" s="788"/>
+      <c r="J77" s="789"/>
       <c r="K77" s="69"/>
       <c r="L77" s="148"/>
       <c r="M77" s="69"/>
@@ -17207,7 +17241,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="751" t="s">
+      <c r="F80" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -17222,7 +17256,7 @@
       <c r="C81" s="462"/>
       <c r="D81" s="463"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="752"/>
+      <c r="F81" s="753"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -17230,10 +17264,10 @@
     </row>
     <row r="82" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="435"/>
-      <c r="B82" s="784" t="s">
+      <c r="B82" s="785" t="s">
         <v>595</v>
       </c>
-      <c r="C82" s="784"/>
+      <c r="C82" s="785"/>
       <c r="I82"/>
       <c r="J82" s="194"/>
     </row>
@@ -17515,23 +17549,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>451</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -17541,24 +17575,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -17573,14 +17607,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -17590,15 +17624,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
-      <c r="W4" s="726" t="s">
+      <c r="R4" s="755"/>
+      <c r="W4" s="727" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="726"/>
+      <c r="X4" s="727"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17649,8 +17683,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="726"/>
-      <c r="X5" s="726"/>
+      <c r="W5" s="727"/>
+      <c r="X5" s="727"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18413,7 +18447,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="730">
+      <c r="W19" s="731">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -18465,7 +18499,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="731"/>
+      <c r="W20" s="732"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -18514,8 +18548,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -18615,8 +18649,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -18671,8 +18705,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -18720,8 +18754,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -18770,8 +18804,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -18819,9 +18853,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18869,9 +18903,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19203,11 +19237,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="745">
+      <c r="M36" s="746">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="747">
+      <c r="N36" s="748">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -19215,7 +19249,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="780">
+      <c r="Q36" s="781">
         <f>SUM(Q5:Q35)</f>
         <v>8.3000000000320142</v>
       </c>
@@ -19240,13 +19274,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="746"/>
-      <c r="N37" s="748"/>
+      <c r="M37" s="747"/>
+      <c r="N37" s="749"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="781"/>
+      <c r="Q37" s="782"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -19296,11 +19330,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="782">
+      <c r="M39" s="783">
         <f>M36+N36</f>
         <v>3054477.02</v>
       </c>
-      <c r="N39" s="783"/>
+      <c r="N39" s="784"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3627989.66</v>
@@ -19928,26 +19962,26 @@
       <c r="A68" s="98"/>
       <c r="B68" s="99"/>
       <c r="C68" s="1"/>
-      <c r="H68" s="700" t="s">
+      <c r="H68" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="701"/>
+      <c r="I68" s="702"/>
       <c r="J68" s="100"/>
-      <c r="K68" s="702">
+      <c r="K68" s="703">
         <f>I66+L66</f>
         <v>314868.39999999997</v>
       </c>
-      <c r="L68" s="735"/>
+      <c r="L68" s="736"/>
       <c r="M68" s="272"/>
       <c r="N68" s="272"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="13"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D69" s="706" t="s">
+      <c r="D69" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="706"/>
+      <c r="E69" s="707"/>
       <c r="F69" s="312">
         <f>F66-K68-C66</f>
         <v>1594593.8500000003</v>
@@ -19956,22 +19990,22 @@
       <c r="J69" s="103"/>
     </row>
     <row r="70" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D70" s="736" t="s">
+      <c r="D70" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="736"/>
+      <c r="E70" s="737"/>
       <c r="F70" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I70" s="707" t="s">
+      <c r="I70" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="708"/>
-      <c r="K70" s="709">
+      <c r="J70" s="709"/>
+      <c r="K70" s="710">
         <f>F72+F73+F74</f>
         <v>1938640.11</v>
       </c>
-      <c r="L70" s="709"/>
+      <c r="L70" s="710"/>
       <c r="M70" s="404"/>
       <c r="N70" s="404"/>
       <c r="O70" s="404"/>
@@ -20012,11 +20046,11 @@
         <v>15</v>
       </c>
       <c r="J72" s="109"/>
-      <c r="K72" s="711">
+      <c r="K72" s="712">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L72" s="712"/>
+      <c r="L72" s="713"/>
     </row>
     <row r="73" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="110" t="s">
@@ -20033,22 +20067,22 @@
       <c r="C74" s="112">
         <v>44647</v>
       </c>
-      <c r="D74" s="689" t="s">
+      <c r="D74" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="690"/>
+      <c r="E74" s="691"/>
       <c r="F74" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I74" s="691" t="s">
+      <c r="I74" s="692" t="s">
         <v>198</v>
       </c>
-      <c r="J74" s="692"/>
-      <c r="K74" s="693">
+      <c r="J74" s="693"/>
+      <c r="K74" s="694">
         <f>K70+K72</f>
         <v>672071.66000000015</v>
       </c>
-      <c r="L74" s="693"/>
+      <c r="L74" s="694"/>
     </row>
     <row r="75" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C75" s="114"/>
@@ -22492,7 +22526,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="751" t="s">
+      <c r="F80" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -22505,7 +22539,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="752"/>
+      <c r="F81" s="753"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -22525,10 +22559,10 @@
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="456"/>
       <c r="B83" s="442"/>
-      <c r="I83" s="789" t="s">
+      <c r="I83" s="790" t="s">
         <v>594</v>
       </c>
-      <c r="J83" s="790"/>
+      <c r="J83" s="791"/>
     </row>
     <row r="84" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="514" t="s">
@@ -22537,8 +22571,8 @@
       <c r="B84" s="515"/>
       <c r="C84" s="516"/>
       <c r="D84" s="491"/>
-      <c r="I84" s="791"/>
-      <c r="J84" s="792"/>
+      <c r="I84" s="792"/>
+      <c r="J84" s="793"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="456"/>
@@ -22810,23 +22844,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -22836,24 +22870,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -22868,14 +22902,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -22885,15 +22919,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
-      <c r="W4" s="726" t="s">
+      <c r="R4" s="755"/>
+      <c r="W4" s="727" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="726"/>
+      <c r="X4" s="727"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22944,8 +22978,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="726"/>
-      <c r="X5" s="726"/>
+      <c r="W5" s="727"/>
+      <c r="X5" s="727"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23704,7 +23738,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="730">
+      <c r="W19" s="731">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -23756,7 +23790,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="731"/>
+      <c r="W20" s="732"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -23805,8 +23839,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -23903,8 +23937,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -23959,8 +23993,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -24006,8 +24040,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -24058,8 +24092,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -24110,9 +24144,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24162,9 +24196,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24768,11 +24802,11 @@
       <c r="L41" s="627">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="745">
+      <c r="M41" s="746">
         <f>SUM(M5:M40)</f>
         <v>2479367.6100000003</v>
       </c>
-      <c r="N41" s="745">
+      <c r="N41" s="746">
         <f>SUM(N5:N40)</f>
         <v>1195667</v>
       </c>
@@ -24780,7 +24814,7 @@
         <f>SUM(P5:P40)</f>
         <v>4355326.74</v>
       </c>
-      <c r="Q41" s="793">
+      <c r="Q41" s="794">
         <f>SUM(Q5:Q40)</f>
         <v>69878.629999999976</v>
       </c>
@@ -24810,10 +24844,10 @@
       <c r="L42" s="630">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="746"/>
-      <c r="N42" s="746"/>
+      <c r="M42" s="747"/>
+      <c r="N42" s="747"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="794"/>
+      <c r="Q42" s="795"/>
     </row>
     <row r="43" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
@@ -24901,11 +24935,11 @@
       <c r="L45" s="627">
         <v>18269.490000000002</v>
       </c>
-      <c r="M45" s="795">
+      <c r="M45" s="796">
         <f>M41+N41</f>
         <v>3675034.6100000003</v>
       </c>
-      <c r="N45" s="796"/>
+      <c r="N45" s="797"/>
       <c r="P45" s="34"/>
       <c r="Q45" s="13"/>
     </row>
@@ -25498,26 +25532,26 @@
       <c r="A70" s="98"/>
       <c r="B70" s="99"/>
       <c r="C70" s="1"/>
-      <c r="H70" s="700" t="s">
+      <c r="H70" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="701"/>
+      <c r="I70" s="702"/>
       <c r="J70" s="100"/>
-      <c r="K70" s="702">
+      <c r="K70" s="703">
         <f>I68+L68</f>
         <v>428155.54000000004</v>
       </c>
-      <c r="L70" s="735"/>
+      <c r="L70" s="736"/>
       <c r="M70" s="272"/>
       <c r="N70" s="272"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="13"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D71" s="706" t="s">
+      <c r="D71" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="706"/>
+      <c r="E71" s="707"/>
       <c r="F71" s="312">
         <f>F68-K70-C68</f>
         <v>1631087.67</v>
@@ -25527,22 +25561,22 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D72" s="736" t="s">
+      <c r="D72" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="736"/>
+      <c r="E72" s="737"/>
       <c r="F72" s="111">
         <v>-1884975.46</v>
       </c>
-      <c r="I72" s="707" t="s">
+      <c r="I72" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J72" s="708"/>
-      <c r="K72" s="709">
+      <c r="J72" s="709"/>
+      <c r="K72" s="710">
         <f>F74+F75+F76</f>
         <v>1777829.89</v>
       </c>
-      <c r="L72" s="709"/>
+      <c r="L72" s="710"/>
       <c r="M72" s="404"/>
       <c r="N72" s="404"/>
       <c r="O72" s="404"/>
@@ -25583,11 +25617,11 @@
         <v>15</v>
       </c>
       <c r="J74" s="109"/>
-      <c r="K74" s="711">
+      <c r="K74" s="712">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L74" s="712"/>
+      <c r="L74" s="713"/>
       <c r="P74" s="34"/>
     </row>
     <row r="75" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25606,22 +25640,22 @@
       <c r="C76" s="112">
         <v>44682</v>
       </c>
-      <c r="D76" s="689" t="s">
+      <c r="D76" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="690"/>
+      <c r="E76" s="691"/>
       <c r="F76" s="113">
         <v>2112071.92</v>
       </c>
-      <c r="I76" s="691" t="s">
+      <c r="I76" s="692" t="s">
         <v>854</v>
       </c>
-      <c r="J76" s="692"/>
-      <c r="K76" s="693">
+      <c r="J76" s="693"/>
+      <c r="K76" s="694">
         <f>K72+K74</f>
         <v>-14987.790000000037</v>
       </c>
-      <c r="L76" s="693"/>
+      <c r="L76" s="694"/>
       <c r="P76" s="34"/>
     </row>
     <row r="77" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
@@ -28326,7 +28360,7 @@
       <c r="C90" s="214"/>
       <c r="D90" s="256"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="751" t="s">
+      <c r="F90" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K90" s="1"/>
@@ -28339,7 +28373,7 @@
       <c r="C91" s="1"/>
       <c r="D91" s="256"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="752"/>
+      <c r="F91" s="753"/>
       <c r="K91" s="1"/>
       <c r="L91" s="97"/>
       <c r="M91" s="3"/>
@@ -28358,10 +28392,10 @@
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="456"/>
       <c r="B93" s="442"/>
-      <c r="I93" s="789" t="s">
+      <c r="I93" s="790" t="s">
         <v>594</v>
       </c>
-      <c r="J93" s="790"/>
+      <c r="J93" s="791"/>
     </row>
     <row r="94" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="456"/>
@@ -28371,8 +28405,8 @@
       <c r="C94" s="518"/>
       <c r="D94" s="519"/>
       <c r="E94" s="520"/>
-      <c r="I94" s="791"/>
-      <c r="J94" s="792"/>
+      <c r="I94" s="792"/>
+      <c r="J94" s="793"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="456"/>
@@ -28813,11 +28847,11 @@
     </row>
     <row r="130" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B130" s="455"/>
-      <c r="C130" s="797">
+      <c r="C130" s="798">
         <f>SUM(D106:D129)</f>
         <v>759581.99999999988</v>
       </c>
-      <c r="D130" s="798"/>
+      <c r="D130" s="799"/>
       <c r="E130" s="257"/>
     </row>
   </sheetData>
@@ -28853,21 +28887,21 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="803" t="s">
+      <c r="F2" s="804" t="s">
         <v>752</v>
       </c>
-      <c r="G2" s="804"/>
-      <c r="H2" s="805"/>
+      <c r="G2" s="805"/>
+      <c r="H2" s="806"/>
     </row>
     <row r="3" spans="2:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="800" t="s">
+      <c r="B3" s="801" t="s">
         <v>748</v>
       </c>
-      <c r="C3" s="801"/>
-      <c r="D3" s="802"/>
-      <c r="F3" s="806"/>
-      <c r="G3" s="807"/>
-      <c r="H3" s="808"/>
+      <c r="C3" s="802"/>
+      <c r="D3" s="803"/>
+      <c r="F3" s="807"/>
+      <c r="G3" s="808"/>
+      <c r="H3" s="809"/>
     </row>
     <row r="4" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="526" t="s">
@@ -29012,11 +29046,11 @@
         <f>SUM(D5:D10)</f>
         <v>264460</v>
       </c>
-      <c r="G11" s="809">
+      <c r="G11" s="810">
         <f>SUM(H5:H10)</f>
         <v>334337</v>
       </c>
-      <c r="H11" s="810"/>
+      <c r="H11" s="811"/>
     </row>
     <row r="13" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="532" t="s">
@@ -29033,23 +29067,23 @@
       <c r="C14" s="532"/>
     </row>
     <row r="15" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="813" t="s">
+      <c r="C15" s="814" t="s">
         <v>750</v>
       </c>
-      <c r="D15" s="811">
+      <c r="D15" s="812">
         <f>D11-D13</f>
         <v>-69877</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="814"/>
-      <c r="D16" s="812"/>
+      <c r="C16" s="815"/>
+      <c r="D16" s="813"/>
     </row>
     <row r="17" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C17" s="799" t="s">
+      <c r="C17" s="800" t="s">
         <v>753</v>
       </c>
-      <c r="D17" s="799"/>
+      <c r="D17" s="800"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -29107,23 +29141,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>754</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -29133,24 +29167,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
       <c r="U3" s="34"/>
@@ -29169,14 +29203,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -29186,15 +29220,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
+      <c r="R4" s="755"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="821"/>
-      <c r="X4" s="821"/>
+      <c r="W4" s="822"/>
+      <c r="X4" s="822"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29248,8 +29282,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="821"/>
-      <c r="X5" s="821"/>
+      <c r="W5" s="822"/>
+      <c r="X5" s="822"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30015,7 +30049,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="822"/>
+      <c r="W19" s="823"/>
       <c r="X19" s="544"/>
       <c r="Y19" s="233"/>
     </row>
@@ -30069,7 +30103,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="822"/>
+      <c r="W20" s="823"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -30124,8 +30158,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -30236,8 +30270,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -30298,8 +30332,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -30352,8 +30386,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -30408,8 +30442,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -30464,9 +30498,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30520,9 +30554,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31113,11 +31147,11 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="745">
+      <c r="M41" s="746">
         <f>SUM(M5:M40)</f>
         <v>1509924.1</v>
       </c>
-      <c r="N41" s="745">
+      <c r="N41" s="746">
         <f>SUM(N5:N40)</f>
         <v>1012291</v>
       </c>
@@ -31125,7 +31159,7 @@
         <f>SUM(P5:P40)</f>
         <v>4043205.8900000006</v>
       </c>
-      <c r="Q41" s="793">
+      <c r="Q41" s="794">
         <f>SUM(Q5:Q40)</f>
         <v>890559.8899999999</v>
       </c>
@@ -31149,10 +31183,10 @@
       <c r="L42" s="640">
         <v>3095.88</v>
       </c>
-      <c r="M42" s="746"/>
-      <c r="N42" s="746"/>
+      <c r="M42" s="747"/>
+      <c r="N42" s="747"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="794"/>
+      <c r="Q42" s="795"/>
     </row>
     <row r="43" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
@@ -31221,11 +31255,11 @@
       <c r="L45" s="619">
         <v>4006.5</v>
       </c>
-      <c r="M45" s="795">
+      <c r="M45" s="796">
         <f>M41+N41</f>
         <v>2522215.1</v>
       </c>
-      <c r="N45" s="796"/>
+      <c r="N45" s="797"/>
       <c r="P45" s="34"/>
       <c r="Q45" s="13"/>
     </row>
@@ -31641,26 +31675,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="700" t="s">
+      <c r="H63" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="701"/>
+      <c r="I63" s="702"/>
       <c r="J63" s="562"/>
-      <c r="K63" s="818">
+      <c r="K63" s="819">
         <f>I61+L61</f>
         <v>340912.75</v>
       </c>
-      <c r="L63" s="819"/>
+      <c r="L63" s="820"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="706" t="s">
+      <c r="D64" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="706"/>
+      <c r="E64" s="707"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>1458827.53</v>
@@ -31669,22 +31703,22 @@
       <c r="J64" s="563"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="736" t="s">
+      <c r="D65" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="736"/>
+      <c r="E65" s="737"/>
       <c r="F65" s="111">
         <v>-1572197.3</v>
       </c>
-      <c r="I65" s="707" t="s">
+      <c r="I65" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="708"/>
-      <c r="K65" s="709">
+      <c r="J65" s="709"/>
+      <c r="K65" s="710">
         <f>F67+F68+F69</f>
         <v>2392765.5300000003</v>
       </c>
-      <c r="L65" s="709"/>
+      <c r="L65" s="710"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="582"/>
@@ -31725,11 +31759,11 @@
         <v>15</v>
       </c>
       <c r="J67" s="109"/>
-      <c r="K67" s="820">
+      <c r="K67" s="821">
         <f>-C4</f>
         <v>-2112071.92</v>
       </c>
-      <c r="L67" s="709"/>
+      <c r="L67" s="710"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -31746,22 +31780,22 @@
       <c r="C69" s="112">
         <v>44710</v>
       </c>
-      <c r="D69" s="689" t="s">
+      <c r="D69" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="690"/>
+      <c r="E69" s="691"/>
       <c r="F69" s="113">
         <v>2546982.16</v>
       </c>
-      <c r="I69" s="815" t="s">
+      <c r="I69" s="816" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="816"/>
-      <c r="K69" s="817">
+      <c r="J69" s="817"/>
+      <c r="K69" s="818">
         <f>K65+K67</f>
         <v>280693.61000000034</v>
       </c>
-      <c r="L69" s="817"/>
+      <c r="L69" s="818"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -33967,7 +34001,7 @@
       <c r="C71" s="214"/>
       <c r="D71" s="256"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="751" t="s">
+      <c r="F71" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K71" s="1"/>
@@ -33980,7 +34014,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="256"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="752"/>
+      <c r="F72" s="753"/>
       <c r="K72" s="1"/>
       <c r="L72" s="97"/>
       <c r="M72" s="3"/>
@@ -33999,10 +34033,10 @@
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="456"/>
       <c r="B74" s="442"/>
-      <c r="I74" s="789" t="s">
+      <c r="I74" s="790" t="s">
         <v>594</v>
       </c>
-      <c r="J74" s="790"/>
+      <c r="J74" s="791"/>
     </row>
     <row r="75" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="456"/>
@@ -34011,8 +34045,8 @@
       <c r="D75" s="654"/>
       <c r="E75" s="520"/>
       <c r="F75" s="111"/>
-      <c r="I75" s="791"/>
-      <c r="J75" s="792"/>
+      <c r="I75" s="792"/>
+      <c r="J75" s="793"/>
     </row>
     <row r="76" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="456"/>
@@ -34146,11 +34180,11 @@
       <c r="N88"/>
     </row>
     <row r="89" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="825" t="s">
+      <c r="A89" s="826" t="s">
         <v>806</v>
       </c>
-      <c r="B89" s="826"/>
-      <c r="C89" s="826"/>
+      <c r="B89" s="827"/>
+      <c r="C89" s="827"/>
       <c r="E89"/>
       <c r="F89" s="111"/>
       <c r="I89"/>
@@ -34160,10 +34194,10 @@
     </row>
     <row r="90" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="454"/>
-      <c r="B90" s="827" t="s">
+      <c r="B90" s="828" t="s">
         <v>807</v>
       </c>
-      <c r="C90" s="828"/>
+      <c r="C90" s="829"/>
       <c r="E90"/>
       <c r="F90" s="111"/>
       <c r="I90"/>
@@ -34264,7 +34298,7 @@
     <row r="97" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97" s="662"/>
-      <c r="C97" s="823">
+      <c r="C97" s="824">
         <f>SUM(C91:C96)</f>
         <v>625124.87</v>
       </c>
@@ -34278,7 +34312,7 @@
       <c r="B98" s="663" t="s">
         <v>883</v>
       </c>
-      <c r="C98" s="824"/>
+      <c r="C98" s="825"/>
       <c r="E98"/>
       <c r="F98" s="127">
         <v>0</v>
@@ -34351,7 +34385,7 @@
   </sheetPr>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
@@ -34378,23 +34412,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>884</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -34404,24 +34438,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -34436,14 +34470,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -34453,11 +34487,11 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
+      <c r="R4" s="755"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -36225,11 +36259,11 @@
       <c r="L41" s="39">
         <v>18992.37</v>
       </c>
-      <c r="M41" s="745">
+      <c r="M41" s="746">
         <f>SUM(M5:M40)</f>
         <v>1737024</v>
       </c>
-      <c r="N41" s="745">
+      <c r="N41" s="746">
         <f>SUM(N5:N40)</f>
         <v>1314313</v>
       </c>
@@ -36237,7 +36271,7 @@
         <f>SUM(P5:P40)</f>
         <v>3810957.55</v>
       </c>
-      <c r="Q41" s="793">
+      <c r="Q41" s="794">
         <f>SUM(Q5:Q40)</f>
         <v>30.55000000000291</v>
       </c>
@@ -36267,10 +36301,10 @@
       <c r="L42" s="52">
         <v>17035.3</v>
       </c>
-      <c r="M42" s="746"/>
-      <c r="N42" s="746"/>
+      <c r="M42" s="747"/>
+      <c r="N42" s="747"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="794"/>
+      <c r="Q42" s="795"/>
     </row>
     <row r="43" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
@@ -36357,11 +36391,11 @@
       <c r="L45" s="39">
         <v>20521</v>
       </c>
-      <c r="M45" s="795">
+      <c r="M45" s="796">
         <f>M41+N41</f>
         <v>3051337</v>
       </c>
-      <c r="N45" s="796"/>
+      <c r="N45" s="797"/>
       <c r="P45" s="34"/>
       <c r="Q45" s="13"/>
     </row>
@@ -36951,26 +36985,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="700" t="s">
+      <c r="H69" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="701"/>
+      <c r="I69" s="702"/>
       <c r="J69" s="562"/>
-      <c r="K69" s="818">
+      <c r="K69" s="819">
         <f>I67+L67</f>
         <v>534683.29</v>
       </c>
-      <c r="L69" s="819"/>
+      <c r="L69" s="820"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="706" t="s">
+      <c r="D70" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="706"/>
+      <c r="E70" s="707"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1683028.8699999999</v>
@@ -36979,22 +37013,22 @@
       <c r="J70" s="563"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="736" t="s">
+      <c r="D71" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="736"/>
+      <c r="E71" s="737"/>
       <c r="F71" s="111">
         <v>-2122394.9</v>
       </c>
-      <c r="I71" s="707" t="s">
+      <c r="I71" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="708"/>
-      <c r="K71" s="709">
+      <c r="J71" s="709"/>
+      <c r="K71" s="710">
         <f>F73+F74+F75</f>
         <v>2167293.46</v>
       </c>
-      <c r="L71" s="709"/>
+      <c r="L71" s="710"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="658"/>
@@ -37035,11 +37069,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="820">
+      <c r="K73" s="821">
         <f>-C4</f>
         <v>-2546982.16</v>
       </c>
-      <c r="L73" s="709"/>
+      <c r="L73" s="710"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -37056,22 +37090,22 @@
       <c r="C75" s="112">
         <v>44745</v>
       </c>
-      <c r="D75" s="689" t="s">
+      <c r="D75" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="690"/>
+      <c r="E75" s="691"/>
       <c r="F75" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I75" s="691" t="s">
+      <c r="I75" s="692" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="692"/>
-      <c r="K75" s="693">
+      <c r="J75" s="693"/>
+      <c r="K75" s="694">
         <f>K71+K73</f>
         <v>-379688.70000000019</v>
       </c>
-      <c r="L75" s="693"/>
+      <c r="L75" s="694"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -37255,7 +37289,7 @@
   </sheetPr>
   <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -39164,10 +39198,10 @@
         <f>SUM(F3:F66)</f>
         <v>1303900.4000000001</v>
       </c>
-      <c r="H67" s="789" t="s">
+      <c r="H67" s="790" t="s">
         <v>594</v>
       </c>
-      <c r="I67" s="790"/>
+      <c r="I67" s="791"/>
       <c r="J67" s="646">
         <f>SUM(J3:J66)</f>
         <v>289475.05</v>
@@ -39187,11 +39221,11 @@
       <c r="C68" s="214"/>
       <c r="D68" s="256"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="751" t="s">
+      <c r="F68" s="752" t="s">
         <v>207</v>
       </c>
-      <c r="H68" s="791"/>
-      <c r="I68" s="792"/>
+      <c r="H68" s="792"/>
+      <c r="I68" s="793"/>
       <c r="J68" s="1"/>
       <c r="K68" s="97"/>
       <c r="L68" s="3"/>
@@ -39202,7 +39236,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="256"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="752"/>
+      <c r="F69" s="753"/>
       <c r="J69" s="1"/>
       <c r="K69" s="97"/>
       <c r="L69" s="3"/>
@@ -41142,7 +41176,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="724" t="s">
+      <c r="B41" s="725" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -41174,7 +41208,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="725"/>
+      <c r="B42" s="726"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -42741,8 +42775,8 @@
   </sheetPr>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -42768,23 +42802,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>1027</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -42794,24 +42828,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -42826,14 +42860,14 @@
       <c r="D4" s="18">
         <v>44745</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -42843,11 +42877,11 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
+      <c r="R4" s="755"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -43474,6 +43508,9 @@
       <c r="N17" s="33">
         <v>54698</v>
       </c>
+      <c r="O17" s="580" t="s">
+        <v>1047</v>
+      </c>
       <c r="P17" s="39">
         <f t="shared" si="1"/>
         <v>130337</v>
@@ -43491,34 +43528,44 @@
       <c r="B18" s="24">
         <v>44759</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="35"/>
+      <c r="C18" s="25">
+        <v>13508</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>1046</v>
+      </c>
       <c r="E18" s="27">
         <v>44759</v>
       </c>
-      <c r="F18" s="28"/>
+      <c r="F18" s="28">
+        <v>128173</v>
+      </c>
       <c r="G18" s="575"/>
       <c r="H18" s="29">
         <v>44759</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="30">
+        <v>1634</v>
+      </c>
       <c r="J18" s="37"/>
       <c r="K18" s="567"/>
       <c r="L18" s="39"/>
       <c r="M18" s="32">
-        <v>0</v>
+        <v>83166</v>
       </c>
       <c r="N18" s="33">
-        <v>0</v>
-      </c>
-      <c r="O18" s="664"/>
+        <v>29065</v>
+      </c>
+      <c r="O18" s="580" t="s">
+        <v>1047</v>
+      </c>
       <c r="P18" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="325">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>127373</v>
+      </c>
+      <c r="Q18" s="386">
+        <f t="shared" si="0"/>
+        <v>-800</v>
       </c>
       <c r="R18" s="319">
         <v>0</v>
@@ -43529,34 +43576,44 @@
       <c r="B19" s="24">
         <v>44760</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="25">
+        <v>15257</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>1048</v>
+      </c>
       <c r="E19" s="27">
         <v>44760</v>
       </c>
-      <c r="F19" s="28"/>
+      <c r="F19" s="28">
+        <v>153702</v>
+      </c>
       <c r="G19" s="575"/>
       <c r="H19" s="29">
         <v>44760</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="30">
+        <v>1745</v>
+      </c>
       <c r="J19" s="37"/>
       <c r="K19" s="46"/>
       <c r="L19" s="47"/>
       <c r="M19" s="32">
-        <v>0</v>
+        <v>92159</v>
       </c>
       <c r="N19" s="33">
-        <v>0</v>
-      </c>
-      <c r="O19" s="664"/>
+        <v>45141</v>
+      </c>
+      <c r="O19" s="580" t="s">
+        <v>1047</v>
+      </c>
       <c r="P19" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>154302</v>
       </c>
       <c r="Q19" s="325">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="R19" s="319">
         <v>0</v>
@@ -43567,34 +43624,44 @@
       <c r="B20" s="24">
         <v>44761</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="35"/>
+      <c r="C20" s="25">
+        <v>5532</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>1049</v>
+      </c>
       <c r="E20" s="27">
         <v>44761</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="28">
+        <v>100478</v>
+      </c>
       <c r="G20" s="575"/>
       <c r="H20" s="29">
         <v>44761</v>
       </c>
-      <c r="I20" s="30"/>
+      <c r="I20" s="30">
+        <v>3379</v>
+      </c>
       <c r="J20" s="37"/>
       <c r="K20" s="171"/>
       <c r="L20" s="45"/>
       <c r="M20" s="32">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="N20" s="33">
-        <v>0</v>
-      </c>
-      <c r="O20" s="664"/>
+        <v>30790</v>
+      </c>
+      <c r="O20" s="661" t="s">
+        <v>1051</v>
+      </c>
       <c r="P20" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="325">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>139701</v>
+      </c>
+      <c r="Q20" s="689">
+        <f t="shared" si="0"/>
+        <v>39223</v>
       </c>
       <c r="R20" s="319">
         <v>0</v>
@@ -43605,34 +43672,45 @@
       <c r="B21" s="24">
         <v>44762</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="25">
+        <v>21598</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>1050</v>
+      </c>
       <c r="E21" s="27">
         <v>44762</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="28">
+        <v>116923</v>
+      </c>
       <c r="G21" s="575"/>
       <c r="H21" s="29">
         <v>44762</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="30">
+        <v>1707</v>
+      </c>
       <c r="J21" s="37"/>
       <c r="K21" s="568"/>
       <c r="L21" s="45"/>
       <c r="M21" s="32">
-        <v>0</v>
+        <f>14700+14714</f>
+        <v>29414</v>
       </c>
       <c r="N21" s="33">
-        <v>0</v>
-      </c>
-      <c r="O21" s="664"/>
+        <v>31157</v>
+      </c>
+      <c r="O21" s="661" t="s">
+        <v>915</v>
+      </c>
       <c r="P21" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="325">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>83876</v>
+      </c>
+      <c r="Q21" s="386">
+        <f t="shared" si="0"/>
+        <v>-33047</v>
       </c>
       <c r="R21" s="319">
         <v>0</v>
@@ -43643,34 +43721,44 @@
       <c r="B22" s="24">
         <v>44763</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="25">
+        <v>7375</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>1052</v>
+      </c>
       <c r="E22" s="27">
         <v>44763</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="28">
+        <v>131922</v>
+      </c>
       <c r="G22" s="575"/>
       <c r="H22" s="29">
         <v>44763</v>
       </c>
-      <c r="I22" s="30"/>
+      <c r="I22" s="30">
+        <v>3065</v>
+      </c>
       <c r="J22" s="37"/>
       <c r="K22" s="31"/>
       <c r="L22" s="49"/>
       <c r="M22" s="32">
-        <v>0</v>
+        <v>80325</v>
       </c>
       <c r="N22" s="33">
-        <v>0</v>
-      </c>
-      <c r="O22" s="664"/>
+        <v>34984</v>
+      </c>
+      <c r="O22" s="664" t="s">
+        <v>766</v>
+      </c>
       <c r="P22" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="325">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125749</v>
+      </c>
+      <c r="Q22" s="386">
+        <f t="shared" si="0"/>
+        <v>-6173</v>
       </c>
       <c r="R22" s="319">
         <v>0</v>
@@ -43681,30 +43769,42 @@
       <c r="B23" s="24">
         <v>44764</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="25">
+        <v>11382</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>1053</v>
+      </c>
       <c r="E23" s="27">
         <v>44764</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="28">
+        <v>80421</v>
+      </c>
       <c r="G23" s="575"/>
       <c r="H23" s="29">
         <v>44764</v>
       </c>
-      <c r="I23" s="30"/>
-      <c r="J23" s="50"/>
+      <c r="I23" s="30">
+        <v>3798</v>
+      </c>
+      <c r="J23" s="50" t="s">
+        <v>7</v>
+      </c>
       <c r="K23" s="172"/>
       <c r="L23" s="45"/>
       <c r="M23" s="32">
-        <v>0</v>
+        <v>40907</v>
       </c>
       <c r="N23" s="33">
-        <v>0</v>
-      </c>
-      <c r="O23" s="664"/>
+        <v>24334</v>
+      </c>
+      <c r="O23" s="664" t="s">
+        <v>766</v>
+      </c>
       <c r="P23" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80421</v>
       </c>
       <c r="Q23" s="325">
         <f t="shared" si="0"/>
@@ -43719,30 +43819,46 @@
       <c r="B24" s="24">
         <v>44765</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="42"/>
+      <c r="C24" s="25">
+        <v>11080.5</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>1054</v>
+      </c>
       <c r="E24" s="27">
         <v>44765</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="28">
+        <v>158449</v>
+      </c>
       <c r="G24" s="575"/>
       <c r="H24" s="29">
         <v>44765</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="173"/>
-      <c r="L24" s="52"/>
+      <c r="I24" s="30">
+        <v>6764</v>
+      </c>
+      <c r="J24" s="51">
+        <v>44765</v>
+      </c>
+      <c r="K24" s="173" t="s">
+        <v>1055</v>
+      </c>
+      <c r="L24" s="52">
+        <v>20533</v>
+      </c>
       <c r="M24" s="32">
-        <v>0</v>
+        <v>72303.5</v>
       </c>
       <c r="N24" s="33">
-        <v>0</v>
-      </c>
-      <c r="O24" s="664"/>
+        <v>47768</v>
+      </c>
+      <c r="O24" s="664" t="s">
+        <v>766</v>
+      </c>
       <c r="P24" s="39">
         <f>N24+M24+L24+I24+C24</f>
-        <v>0</v>
+        <v>158449</v>
       </c>
       <c r="Q24" s="325">
         <f t="shared" si="0"/>
@@ -43815,7 +43931,7 @@
       <c r="N26" s="33">
         <v>0</v>
       </c>
-      <c r="P26" s="284">
+      <c r="P26" s="283">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -43852,7 +43968,7 @@
       <c r="N27" s="33">
         <v>0</v>
       </c>
-      <c r="P27" s="39">
+      <c r="P27" s="283">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -43889,7 +44005,7 @@
       <c r="N28" s="33">
         <v>0</v>
       </c>
-      <c r="P28" s="34">
+      <c r="P28" s="283">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -43926,7 +44042,7 @@
       <c r="N29" s="33">
         <v>0</v>
       </c>
-      <c r="P29" s="34">
+      <c r="P29" s="283">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -43963,7 +44079,7 @@
       <c r="N30" s="33">
         <v>0</v>
       </c>
-      <c r="P30" s="34">
+      <c r="P30" s="283">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -44106,12 +44222,11 @@
         <v>0</v>
       </c>
       <c r="P34" s="34">
-        <f t="shared" si="1"/>
-        <v>19463.41</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="325">
         <f t="shared" si="0"/>
-        <v>19463.41</v>
+        <v>0</v>
       </c>
       <c r="R34" s="319">
         <v>0</v>
@@ -44143,12 +44258,11 @@
         <v>0</v>
       </c>
       <c r="P35" s="34">
-        <f t="shared" si="1"/>
-        <v>19849.560000000001</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="325">
         <f t="shared" si="0"/>
-        <v>19849.560000000001</v>
+        <v>0</v>
       </c>
       <c r="R35" s="319">
         <v>0</v>
@@ -44164,9 +44278,15 @@
       <c r="G36" s="666"/>
       <c r="H36" s="29"/>
       <c r="I36" s="30"/>
-      <c r="J36" s="560"/>
-      <c r="K36" s="572"/>
-      <c r="L36" s="9"/>
+      <c r="J36" s="560">
+        <v>44765</v>
+      </c>
+      <c r="K36" s="572" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L36" s="9">
+        <v>18868</v>
+      </c>
       <c r="M36" s="32">
         <v>0</v>
       </c>
@@ -44174,7 +44294,6 @@
         <v>0</v>
       </c>
       <c r="P36" s="34">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q36" s="325">
@@ -44322,21 +44441,21 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="745">
+      <c r="M41" s="746">
         <f>SUM(M5:M40)</f>
-        <v>602480.5</v>
-      </c>
-      <c r="N41" s="745">
+        <v>1100755</v>
+      </c>
+      <c r="N41" s="746">
         <f>SUM(N5:N40)</f>
-        <v>500173</v>
+        <v>743412</v>
       </c>
       <c r="P41" s="506">
         <f>SUM(P5:P40)</f>
-        <v>1480306.97</v>
-      </c>
-      <c r="Q41" s="793">
+        <v>2310865</v>
+      </c>
+      <c r="Q41" s="794">
         <f>SUM(Q5:Q40)</f>
-        <v>39521.97</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -44352,10 +44471,10 @@
       <c r="J42" s="51"/>
       <c r="K42" s="173"/>
       <c r="L42" s="52"/>
-      <c r="M42" s="746"/>
-      <c r="N42" s="746"/>
+      <c r="M42" s="747"/>
+      <c r="N42" s="747"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="794"/>
+      <c r="Q42" s="795"/>
     </row>
     <row r="43" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
@@ -44406,11 +44525,11 @@
       <c r="J45" s="56"/>
       <c r="K45" s="38"/>
       <c r="L45" s="39"/>
-      <c r="M45" s="795">
+      <c r="M45" s="796">
         <f>M41+N41</f>
-        <v>1102653.5</v>
-      </c>
-      <c r="N45" s="796"/>
+        <v>1844167</v>
+      </c>
+      <c r="N45" s="797"/>
       <c r="P45" s="34"/>
       <c r="Q45" s="13"/>
     </row>
@@ -44807,7 +44926,7 @@
       </c>
       <c r="C67" s="87">
         <f>SUM(C5:C60)</f>
-        <v>255465.5</v>
+        <v>341198</v>
       </c>
       <c r="D67" s="88"/>
       <c r="E67" s="91" t="s">
@@ -44815,7 +44934,7 @@
       </c>
       <c r="F67" s="90">
         <f>SUM(F5:F60)</f>
-        <v>1375208</v>
+        <v>2245276</v>
       </c>
       <c r="G67" s="576"/>
       <c r="H67" s="91" t="s">
@@ -44823,7 +44942,7 @@
       </c>
       <c r="I67" s="92">
         <f>SUM(I5:I60)</f>
-        <v>45168</v>
+        <v>67260</v>
       </c>
       <c r="J67" s="93"/>
       <c r="K67" s="94" t="s">
@@ -44831,7 +44950,7 @@
       </c>
       <c r="L67" s="95">
         <f>SUM(L5:L65)</f>
-        <v>77019.97</v>
+        <v>116420.97</v>
       </c>
       <c r="M67" s="96"/>
       <c r="N67" s="96"/>
@@ -44849,50 +44968,50 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="700" t="s">
+      <c r="H69" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="701"/>
+      <c r="I69" s="702"/>
       <c r="J69" s="562"/>
-      <c r="K69" s="818">
+      <c r="K69" s="819">
         <f>I67+L67</f>
-        <v>122187.97</v>
-      </c>
-      <c r="L69" s="819"/>
+        <v>183680.97</v>
+      </c>
+      <c r="L69" s="820"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="706" t="s">
+      <c r="D70" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="706"/>
+      <c r="E70" s="707"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
-        <v>997554.53</v>
+        <v>1720397.03</v>
       </c>
       <c r="I70" s="102"/>
       <c r="J70" s="563"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="736" t="s">
+      <c r="D71" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="736"/>
+      <c r="E71" s="737"/>
       <c r="F71" s="111">
         <v>0</v>
       </c>
-      <c r="I71" s="707" t="s">
+      <c r="I71" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="708"/>
-      <c r="K71" s="709">
+      <c r="J71" s="709"/>
+      <c r="K71" s="710">
         <f>F73+F74+F75</f>
-        <v>3352981.0700000003</v>
-      </c>
-      <c r="L71" s="709"/>
+        <v>4075823.5700000003</v>
+      </c>
+      <c r="L71" s="710"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="658"/>
@@ -44926,18 +45045,18 @@
       </c>
       <c r="F73" s="96">
         <f>SUM(F70:F72)</f>
-        <v>997554.53</v>
+        <v>1720397.03</v>
       </c>
       <c r="H73" s="558"/>
       <c r="I73" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="820">
+      <c r="K73" s="821">
         <f>-C4</f>
         <v>-2355426.54</v>
       </c>
-      <c r="L73" s="709"/>
+      <c r="L73" s="710"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -44952,22 +45071,22 @@
     </row>
     <row r="75" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="112"/>
-      <c r="D75" s="689" t="s">
+      <c r="D75" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="690"/>
+      <c r="E75" s="691"/>
       <c r="F75" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I75" s="691" t="s">
+      <c r="I75" s="692" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="692"/>
-      <c r="K75" s="693">
+      <c r="J75" s="693"/>
+      <c r="K75" s="694">
         <f>K71+K73</f>
-        <v>997554.53000000026</v>
-      </c>
-      <c r="L75" s="693"/>
+        <v>1720397.0300000003</v>
+      </c>
+      <c r="L75" s="694"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -46537,10 +46656,10 @@
         <f>SUM(F3:F66)</f>
         <v>0</v>
       </c>
-      <c r="H67" s="789" t="s">
+      <c r="H67" s="790" t="s">
         <v>594</v>
       </c>
-      <c r="I67" s="790"/>
+      <c r="I67" s="791"/>
       <c r="J67" s="646">
         <f>SUM(J3:J66)</f>
         <v>0</v>
@@ -46560,11 +46679,11 @@
       <c r="C68" s="214"/>
       <c r="D68" s="256"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="751" t="s">
+      <c r="F68" s="752" t="s">
         <v>207</v>
       </c>
-      <c r="H68" s="791"/>
-      <c r="I68" s="792"/>
+      <c r="H68" s="792"/>
+      <c r="I68" s="793"/>
       <c r="J68" s="1"/>
       <c r="K68" s="97"/>
       <c r="L68" s="3"/>
@@ -46575,7 +46694,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="256"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="752"/>
+      <c r="F69" s="753"/>
       <c r="J69" s="1"/>
       <c r="K69" s="97"/>
       <c r="L69" s="3"/>
@@ -47243,23 +47362,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="715" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="716" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="716"/>
-      <c r="E1" s="716"/>
-      <c r="F1" s="716"/>
-      <c r="G1" s="716"/>
-      <c r="H1" s="716"/>
-      <c r="I1" s="716"/>
-      <c r="J1" s="716"/>
-      <c r="K1" s="716"/>
-      <c r="L1" s="716"/>
-      <c r="M1" s="716"/>
+      <c r="D1" s="717"/>
+      <c r="E1" s="717"/>
+      <c r="F1" s="717"/>
+      <c r="G1" s="717"/>
+      <c r="H1" s="717"/>
+      <c r="I1" s="717"/>
+      <c r="J1" s="717"/>
+      <c r="K1" s="717"/>
+      <c r="L1" s="717"/>
+      <c r="M1" s="717"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -47269,21 +47388,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
     </row>
@@ -47298,14 +47417,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -47315,14 +47434,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="726" t="s">
+      <c r="W4" s="727" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="726"/>
+      <c r="X4" s="727"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47373,8 +47492,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="726"/>
-      <c r="X5" s="726"/>
+      <c r="W5" s="727"/>
+      <c r="X5" s="727"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48145,7 +48264,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="730">
+      <c r="W19" s="731">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -48197,7 +48316,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="731"/>
+      <c r="W20" s="732"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -48246,8 +48365,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -48348,8 +48467,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -48403,8 +48522,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -48450,8 +48569,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -48502,8 +48621,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -48551,9 +48670,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48603,9 +48722,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48940,11 +49059,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="745">
+      <c r="M36" s="746">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="747">
+      <c r="N36" s="748">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -48952,7 +49071,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="749">
+      <c r="Q36" s="750">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -48987,13 +49106,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="746"/>
-      <c r="N37" s="748"/>
+      <c r="M37" s="747"/>
+      <c r="N37" s="749"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="750"/>
+      <c r="Q37" s="751"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -49283,26 +49402,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="700" t="s">
+      <c r="H52" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="701"/>
+      <c r="I52" s="702"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="702">
+      <c r="K52" s="703">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="735"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="706" t="s">
+      <c r="D53" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="706"/>
+      <c r="E53" s="707"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -49311,29 +49430,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="736" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="736"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="707" t="s">
+      <c r="I54" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="708"/>
-      <c r="K54" s="709">
+      <c r="J54" s="709"/>
+      <c r="K54" s="710">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="709"/>
-      <c r="M54" s="737" t="s">
+      <c r="L54" s="710"/>
+      <c r="M54" s="738" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="738"/>
-      <c r="O54" s="738"/>
-      <c r="P54" s="738"/>
-      <c r="Q54" s="739"/>
+      <c r="N54" s="739"/>
+      <c r="O54" s="739"/>
+      <c r="P54" s="739"/>
+      <c r="Q54" s="740"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -49347,11 +49466,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="740"/>
-      <c r="N55" s="741"/>
-      <c r="O55" s="741"/>
-      <c r="P55" s="741"/>
-      <c r="Q55" s="742"/>
+      <c r="M55" s="741"/>
+      <c r="N55" s="742"/>
+      <c r="O55" s="742"/>
+      <c r="P55" s="742"/>
+      <c r="Q55" s="743"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -49369,11 +49488,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="711">
+      <c r="K56" s="712">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="712"/>
+      <c r="L56" s="713"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -49390,22 +49509,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="689" t="s">
+      <c r="D58" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="690"/>
+      <c r="E58" s="691"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="691" t="s">
+      <c r="I58" s="692" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="692"/>
-      <c r="K58" s="693">
+      <c r="J58" s="693"/>
+      <c r="K58" s="694">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="693"/>
+      <c r="L58" s="694"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -51995,7 +52114,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="751" t="s">
+      <c r="F87" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -52008,7 +52127,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="752"/>
+      <c r="F88" s="753"/>
       <c r="K88" s="1"/>
       <c r="L88" s="256"/>
       <c r="M88" s="3"/>
@@ -52320,23 +52439,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="715" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="716" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="716"/>
-      <c r="E1" s="716"/>
-      <c r="F1" s="716"/>
-      <c r="G1" s="716"/>
-      <c r="H1" s="716"/>
-      <c r="I1" s="716"/>
-      <c r="J1" s="716"/>
-      <c r="K1" s="716"/>
-      <c r="L1" s="716"/>
-      <c r="M1" s="716"/>
+      <c r="D1" s="717"/>
+      <c r="E1" s="717"/>
+      <c r="F1" s="717"/>
+      <c r="G1" s="717"/>
+      <c r="H1" s="717"/>
+      <c r="I1" s="717"/>
+      <c r="J1" s="717"/>
+      <c r="K1" s="717"/>
+      <c r="L1" s="717"/>
+      <c r="M1" s="717"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -52346,24 +52465,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -52378,14 +52497,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -52395,15 +52514,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
-      <c r="W4" s="726" t="s">
+      <c r="R4" s="755"/>
+      <c r="W4" s="727" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="726"/>
+      <c r="X4" s="727"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52464,8 +52583,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="726"/>
-      <c r="X5" s="726"/>
+      <c r="W5" s="727"/>
+      <c r="X5" s="727"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -53222,7 +53341,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="730">
+      <c r="W19" s="731">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -53274,7 +53393,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="731"/>
+      <c r="W20" s="732"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -53323,8 +53442,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -53425,8 +53544,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -53477,8 +53596,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -53524,8 +53643,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -53573,8 +53692,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -53634,9 +53753,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -53690,9 +53809,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -54008,11 +54127,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="745">
+      <c r="M36" s="746">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="747">
+      <c r="N36" s="748">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -54020,7 +54139,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="749">
+      <c r="Q36" s="750">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -54039,13 +54158,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="746"/>
-      <c r="N37" s="748"/>
+      <c r="M37" s="747"/>
+      <c r="N37" s="749"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="750"/>
+      <c r="Q37" s="751"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -54319,26 +54438,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="700" t="s">
+      <c r="H52" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="701"/>
+      <c r="I52" s="702"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="702">
+      <c r="K52" s="703">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="735"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="706" t="s">
+      <c r="D53" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="706"/>
+      <c r="E53" s="707"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -54347,29 +54466,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="736" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="736"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="707" t="s">
+      <c r="I54" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="708"/>
-      <c r="K54" s="709">
+      <c r="J54" s="709"/>
+      <c r="K54" s="710">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="709"/>
-      <c r="M54" s="737" t="s">
+      <c r="L54" s="710"/>
+      <c r="M54" s="738" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="738"/>
-      <c r="O54" s="738"/>
-      <c r="P54" s="738"/>
-      <c r="Q54" s="739"/>
+      <c r="N54" s="739"/>
+      <c r="O54" s="739"/>
+      <c r="P54" s="739"/>
+      <c r="Q54" s="740"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -54383,11 +54502,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="740"/>
-      <c r="N55" s="741"/>
-      <c r="O55" s="741"/>
-      <c r="P55" s="741"/>
-      <c r="Q55" s="742"/>
+      <c r="M55" s="741"/>
+      <c r="N55" s="742"/>
+      <c r="O55" s="742"/>
+      <c r="P55" s="742"/>
+      <c r="Q55" s="743"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -54405,11 +54524,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="711">
+      <c r="K56" s="712">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="712"/>
+      <c r="L56" s="713"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -54426,22 +54545,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="689" t="s">
+      <c r="D58" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="690"/>
+      <c r="E58" s="691"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="691" t="s">
+      <c r="I58" s="692" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="692"/>
-      <c r="K58" s="693">
+      <c r="J58" s="693"/>
+      <c r="K58" s="694">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="693"/>
+      <c r="L58" s="694"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -57004,7 +57123,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="256"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="751" t="s">
+      <c r="F75" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -57017,7 +57136,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="256"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="752"/>
+      <c r="F76" s="753"/>
       <c r="K76" s="1"/>
       <c r="L76" s="256"/>
       <c r="M76" s="3"/>
@@ -57309,23 +57428,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -57335,24 +57454,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -57367,14 +57486,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -57384,15 +57503,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
-      <c r="W4" s="726" t="s">
+      <c r="R4" s="755"/>
+      <c r="W4" s="727" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="726"/>
+      <c r="X4" s="727"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57443,8 +57562,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="726"/>
-      <c r="X5" s="726"/>
+      <c r="W5" s="727"/>
+      <c r="X5" s="727"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58208,7 +58327,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="730">
+      <c r="W19" s="731">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -58261,7 +58380,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="731"/>
+      <c r="W20" s="732"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -58310,8 +58429,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -58411,8 +58530,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -58467,8 +58586,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -58513,8 +58632,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -58562,8 +58681,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -58617,9 +58736,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58673,9 +58792,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58986,11 +59105,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="745">
+      <c r="M36" s="746">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="747">
+      <c r="N36" s="748">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -58998,7 +59117,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="749">
+      <c r="Q36" s="750">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -59023,13 +59142,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="746"/>
-      <c r="N37" s="748"/>
+      <c r="M37" s="747"/>
+      <c r="N37" s="749"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="750"/>
+      <c r="Q37" s="751"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -59322,26 +59441,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="700" t="s">
+      <c r="H52" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="701"/>
+      <c r="I52" s="702"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="702">
+      <c r="K52" s="703">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="735"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="706" t="s">
+      <c r="D53" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="706"/>
+      <c r="E53" s="707"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -59350,22 +59469,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="736" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="736"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="707" t="s">
+      <c r="I54" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="708"/>
-      <c r="K54" s="709">
+      <c r="J54" s="709"/>
+      <c r="K54" s="710">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="709"/>
+      <c r="L54" s="710"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -59406,11 +59525,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="711">
+      <c r="K56" s="712">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="712"/>
+      <c r="L56" s="713"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -59427,22 +59546,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="689" t="s">
+      <c r="D58" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="690"/>
+      <c r="E58" s="691"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="691" t="s">
+      <c r="I58" s="692" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="692"/>
-      <c r="K58" s="693">
+      <c r="J58" s="693"/>
+      <c r="K58" s="694">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="693"/>
+      <c r="L58" s="694"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -61311,12 +61430,12 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="245"/>
-      <c r="B43" s="757" t="s">
+      <c r="B43" s="758" t="s">
         <v>413</v>
       </c>
-      <c r="C43" s="758"/>
-      <c r="D43" s="758"/>
-      <c r="E43" s="759"/>
+      <c r="C43" s="759"/>
+      <c r="D43" s="759"/>
+      <c r="E43" s="760"/>
       <c r="F43" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -61344,10 +61463,10 @@
     </row>
     <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="245"/>
-      <c r="B44" s="760"/>
-      <c r="C44" s="761"/>
-      <c r="D44" s="761"/>
-      <c r="E44" s="762"/>
+      <c r="B44" s="761"/>
+      <c r="C44" s="762"/>
+      <c r="D44" s="762"/>
+      <c r="E44" s="763"/>
       <c r="F44" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -61375,10 +61494,10 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="245"/>
-      <c r="B45" s="763"/>
-      <c r="C45" s="764"/>
-      <c r="D45" s="764"/>
-      <c r="E45" s="765"/>
+      <c r="B45" s="764"/>
+      <c r="C45" s="765"/>
+      <c r="D45" s="765"/>
+      <c r="E45" s="766"/>
       <c r="F45" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -61421,10 +61540,10 @@
     </row>
     <row r="47" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="245"/>
-      <c r="B47" s="772" t="s">
+      <c r="B47" s="773" t="s">
         <v>593</v>
       </c>
-      <c r="C47" s="773"/>
+      <c r="C47" s="774"/>
       <c r="D47" s="253"/>
       <c r="E47" s="69"/>
       <c r="F47" s="137">
@@ -61446,8 +61565,8 @@
     </row>
     <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="245"/>
-      <c r="B48" s="774"/>
-      <c r="C48" s="775"/>
+      <c r="B48" s="775"/>
+      <c r="C48" s="776"/>
       <c r="D48" s="253"/>
       <c r="E48" s="69"/>
       <c r="F48" s="137">
@@ -61455,11 +61574,11 @@
         <v>0</v>
       </c>
       <c r="I48" s="348"/>
-      <c r="J48" s="766" t="s">
+      <c r="J48" s="767" t="s">
         <v>414</v>
       </c>
-      <c r="K48" s="767"/>
-      <c r="L48" s="768"/>
+      <c r="K48" s="768"/>
+      <c r="L48" s="769"/>
       <c r="M48" s="206"/>
       <c r="N48" s="137">
         <f>N47+K48-M48</f>
@@ -61477,9 +61596,9 @@
         <v>0</v>
       </c>
       <c r="I49" s="348"/>
-      <c r="J49" s="769"/>
-      <c r="K49" s="770"/>
-      <c r="L49" s="771"/>
+      <c r="J49" s="770"/>
+      <c r="K49" s="771"/>
+      <c r="L49" s="772"/>
       <c r="M49" s="206"/>
       <c r="N49" s="137">
         <f t="shared" si="1"/>
@@ -61496,10 +61615,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I50" s="776" t="s">
+      <c r="I50" s="777" t="s">
         <v>594</v>
       </c>
-      <c r="J50" s="777"/>
+      <c r="J50" s="778"/>
       <c r="K50" s="215">
         <v>0</v>
       </c>
@@ -61520,8 +61639,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I51" s="776"/>
-      <c r="J51" s="777"/>
+      <c r="I51" s="777"/>
+      <c r="J51" s="778"/>
       <c r="K51" s="69"/>
       <c r="L51" s="253"/>
       <c r="M51" s="69"/>
@@ -61540,8 +61659,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I52" s="776"/>
-      <c r="J52" s="777"/>
+      <c r="I52" s="777"/>
+      <c r="J52" s="778"/>
       <c r="K52" s="69"/>
       <c r="L52" s="253"/>
       <c r="M52" s="69"/>
@@ -61560,8 +61679,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I53" s="776"/>
-      <c r="J53" s="777"/>
+      <c r="I53" s="777"/>
+      <c r="J53" s="778"/>
       <c r="K53" s="69"/>
       <c r="L53" s="253"/>
       <c r="M53" s="69"/>
@@ -61580,8 +61699,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I54" s="776"/>
-      <c r="J54" s="777"/>
+      <c r="I54" s="777"/>
+      <c r="J54" s="778"/>
       <c r="K54" s="69"/>
       <c r="L54" s="253"/>
       <c r="M54" s="69"/>
@@ -61600,8 +61719,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I55" s="776"/>
-      <c r="J55" s="777"/>
+      <c r="I55" s="777"/>
+      <c r="J55" s="778"/>
       <c r="K55" s="69"/>
       <c r="L55" s="253"/>
       <c r="M55" s="69"/>
@@ -61620,8 +61739,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I56" s="776"/>
-      <c r="J56" s="777"/>
+      <c r="I56" s="777"/>
+      <c r="J56" s="778"/>
       <c r="K56" s="69"/>
       <c r="L56" s="253"/>
       <c r="M56" s="69"/>
@@ -61640,8 +61759,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I57" s="776"/>
-      <c r="J57" s="777"/>
+      <c r="I57" s="777"/>
+      <c r="J57" s="778"/>
       <c r="K57" s="69"/>
       <c r="L57" s="253"/>
       <c r="M57" s="69"/>
@@ -61660,8 +61779,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I58" s="776"/>
-      <c r="J58" s="777"/>
+      <c r="I58" s="777"/>
+      <c r="J58" s="778"/>
       <c r="K58" s="69"/>
       <c r="L58" s="253"/>
       <c r="M58" s="69"/>
@@ -61680,8 +61799,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I59" s="776"/>
-      <c r="J59" s="777"/>
+      <c r="I59" s="777"/>
+      <c r="J59" s="778"/>
       <c r="K59" s="69"/>
       <c r="L59" s="253"/>
       <c r="M59" s="69"/>
@@ -61700,8 +61819,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I60" s="776"/>
-      <c r="J60" s="777"/>
+      <c r="I60" s="777"/>
+      <c r="J60" s="778"/>
       <c r="K60" s="69"/>
       <c r="L60" s="253"/>
       <c r="M60" s="69"/>
@@ -61720,8 +61839,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I61" s="776"/>
-      <c r="J61" s="777"/>
+      <c r="I61" s="777"/>
+      <c r="J61" s="778"/>
       <c r="K61" s="69"/>
       <c r="L61" s="253"/>
       <c r="M61" s="69"/>
@@ -61740,8 +61859,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I62" s="776"/>
-      <c r="J62" s="777"/>
+      <c r="I62" s="777"/>
+      <c r="J62" s="778"/>
       <c r="K62" s="34"/>
       <c r="L62" s="118"/>
       <c r="M62" s="34"/>
@@ -61760,8 +61879,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I63" s="776"/>
-      <c r="J63" s="777"/>
+      <c r="I63" s="777"/>
+      <c r="J63" s="778"/>
       <c r="K63" s="34"/>
       <c r="L63" s="118"/>
       <c r="M63" s="34"/>
@@ -61780,8 +61899,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I64" s="776"/>
-      <c r="J64" s="777"/>
+      <c r="I64" s="777"/>
+      <c r="J64" s="778"/>
       <c r="K64" s="34"/>
       <c r="L64" s="118"/>
       <c r="M64" s="34"/>
@@ -61800,8 +61919,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I65" s="776"/>
-      <c r="J65" s="777"/>
+      <c r="I65" s="777"/>
+      <c r="J65" s="778"/>
       <c r="K65" s="34"/>
       <c r="L65" s="118"/>
       <c r="M65" s="34"/>
@@ -61820,8 +61939,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I66" s="776"/>
-      <c r="J66" s="777"/>
+      <c r="I66" s="777"/>
+      <c r="J66" s="778"/>
       <c r="K66" s="34"/>
       <c r="L66" s="118"/>
       <c r="M66" s="34"/>
@@ -61840,8 +61959,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I67" s="776"/>
-      <c r="J67" s="777"/>
+      <c r="I67" s="777"/>
+      <c r="J67" s="778"/>
       <c r="K67" s="34"/>
       <c r="L67" s="118"/>
       <c r="M67" s="34"/>
@@ -61860,8 +61979,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I68" s="776"/>
-      <c r="J68" s="777"/>
+      <c r="I68" s="777"/>
+      <c r="J68" s="778"/>
       <c r="K68" s="69"/>
       <c r="L68" s="254"/>
       <c r="M68" s="69"/>
@@ -61880,8 +61999,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I69" s="776"/>
-      <c r="J69" s="777"/>
+      <c r="I69" s="777"/>
+      <c r="J69" s="778"/>
       <c r="K69" s="69"/>
       <c r="L69" s="254"/>
       <c r="M69" s="69"/>
@@ -61900,8 +62019,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I70" s="776"/>
-      <c r="J70" s="777"/>
+      <c r="I70" s="777"/>
+      <c r="J70" s="778"/>
       <c r="K70" s="69"/>
       <c r="L70" s="254"/>
       <c r="M70" s="69"/>
@@ -61920,8 +62039,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I71" s="776"/>
-      <c r="J71" s="777"/>
+      <c r="I71" s="777"/>
+      <c r="J71" s="778"/>
       <c r="K71" s="69"/>
       <c r="L71" s="254"/>
       <c r="M71" s="69"/>
@@ -61940,8 +62059,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I72" s="776"/>
-      <c r="J72" s="777"/>
+      <c r="I72" s="777"/>
+      <c r="J72" s="778"/>
       <c r="K72" s="69"/>
       <c r="L72" s="254"/>
       <c r="M72" s="69"/>
@@ -61960,8 +62079,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I73" s="776"/>
-      <c r="J73" s="777"/>
+      <c r="I73" s="777"/>
+      <c r="J73" s="778"/>
       <c r="K73" s="69"/>
       <c r="L73" s="254"/>
       <c r="M73" s="69"/>
@@ -61980,8 +62099,8 @@
         <f>F73+C74-E74</f>
         <v>0</v>
       </c>
-      <c r="I74" s="776"/>
-      <c r="J74" s="777"/>
+      <c r="I74" s="777"/>
+      <c r="J74" s="778"/>
       <c r="K74" s="69"/>
       <c r="L74" s="254"/>
       <c r="M74" s="69"/>
@@ -62000,8 +62119,8 @@
         <f>F74+C75-E75</f>
         <v>0</v>
       </c>
-      <c r="I75" s="776"/>
-      <c r="J75" s="777"/>
+      <c r="I75" s="777"/>
+      <c r="J75" s="778"/>
       <c r="K75" s="69"/>
       <c r="L75" s="254"/>
       <c r="M75" s="69"/>
@@ -62020,8 +62139,8 @@
         <f>F75+C76-E76</f>
         <v>0</v>
       </c>
-      <c r="I76" s="776"/>
-      <c r="J76" s="777"/>
+      <c r="I76" s="777"/>
+      <c r="J76" s="778"/>
       <c r="K76" s="69"/>
       <c r="L76" s="254"/>
       <c r="M76" s="69"/>
@@ -62040,8 +62159,8 @@
         <f>F76+C77-E77</f>
         <v>0</v>
       </c>
-      <c r="I77" s="776"/>
-      <c r="J77" s="777"/>
+      <c r="I77" s="777"/>
+      <c r="J77" s="778"/>
       <c r="K77" s="69"/>
       <c r="L77" s="254"/>
       <c r="M77" s="69"/>
@@ -62062,8 +62181,8 @@
         <f>F77+C78-E78</f>
         <v>0</v>
       </c>
-      <c r="I78" s="778"/>
-      <c r="J78" s="779"/>
+      <c r="I78" s="779"/>
+      <c r="J78" s="780"/>
       <c r="K78" s="151">
         <v>0</v>
       </c>
@@ -62108,7 +62227,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="751" t="s">
+      <c r="F80" s="752" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -62120,7 +62239,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="752"/>
+      <c r="F81" s="753"/>
       <c r="K81" s="1"/>
       <c r="M81" s="3"/>
       <c r="N81" s="1"/>
@@ -62408,23 +62527,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="713"/>
-      <c r="C1" s="755" t="s">
+      <c r="B1" s="714"/>
+      <c r="C1" s="756" t="s">
         <v>646</v>
       </c>
-      <c r="D1" s="756"/>
-      <c r="E1" s="756"/>
-      <c r="F1" s="756"/>
-      <c r="G1" s="756"/>
-      <c r="H1" s="756"/>
-      <c r="I1" s="756"/>
-      <c r="J1" s="756"/>
-      <c r="K1" s="756"/>
-      <c r="L1" s="756"/>
-      <c r="M1" s="756"/>
+      <c r="D1" s="757"/>
+      <c r="E1" s="757"/>
+      <c r="F1" s="757"/>
+      <c r="G1" s="757"/>
+      <c r="H1" s="757"/>
+      <c r="I1" s="757"/>
+      <c r="J1" s="757"/>
+      <c r="K1" s="757"/>
+      <c r="L1" s="757"/>
+      <c r="M1" s="757"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="714"/>
+      <c r="B2" s="715"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -62434,24 +62553,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="717" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="718"/>
+      <c r="B3" s="718" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="719"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="719" t="s">
+      <c r="H3" s="720" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="719"/>
+      <c r="I3" s="720"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="743" t="s">
+      <c r="P3" s="744" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="753" t="s">
+      <c r="R3" s="754" t="s">
         <v>216</v>
       </c>
     </row>
@@ -62466,14 +62585,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="720" t="s">
+      <c r="E4" s="721" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="721"/>
-      <c r="H4" s="722" t="s">
+      <c r="F4" s="722"/>
+      <c r="H4" s="723" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="723"/>
+      <c r="I4" s="724"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -62483,15 +62602,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="744"/>
+      <c r="P4" s="745"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="754"/>
-      <c r="W4" s="726" t="s">
+      <c r="R4" s="755"/>
+      <c r="W4" s="727" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="726"/>
+      <c r="X4" s="727"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -62542,8 +62661,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="726"/>
-      <c r="X5" s="726"/>
+      <c r="W5" s="727"/>
+      <c r="X5" s="727"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -63304,7 +63423,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="730">
+      <c r="W19" s="731">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -63356,7 +63475,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="731"/>
+      <c r="W20" s="732"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -63405,8 +63524,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="732"/>
-      <c r="X21" s="732"/>
+      <c r="W21" s="733"/>
+      <c r="X21" s="733"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -63505,8 +63624,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="733"/>
-      <c r="X23" s="733"/>
+      <c r="W23" s="734"/>
+      <c r="X23" s="734"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -63561,8 +63680,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="733"/>
-      <c r="X24" s="733"/>
+      <c r="W24" s="734"/>
+      <c r="X24" s="734"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -63610,8 +63729,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="734"/>
-      <c r="X25" s="734"/>
+      <c r="W25" s="735"/>
+      <c r="X25" s="735"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -63659,8 +63778,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="734"/>
-      <c r="X26" s="734"/>
+      <c r="W26" s="735"/>
+      <c r="X26" s="735"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -63708,9 +63827,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="727"/>
-      <c r="X27" s="728"/>
-      <c r="Y27" s="729"/>
+      <c r="W27" s="728"/>
+      <c r="X27" s="729"/>
+      <c r="Y27" s="730"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -63758,9 +63877,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="728"/>
-      <c r="X28" s="728"/>
-      <c r="Y28" s="729"/>
+      <c r="W28" s="729"/>
+      <c r="X28" s="729"/>
+      <c r="Y28" s="730"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -64101,11 +64220,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="745">
+      <c r="M36" s="746">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="747">
+      <c r="N36" s="748">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -64113,7 +64232,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="780">
+      <c r="Q36" s="781">
         <f>SUM(Q5:Q35)</f>
         <v>111.43999999999505</v>
       </c>
@@ -64138,13 +64257,13 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="746"/>
-      <c r="N37" s="748"/>
+      <c r="M37" s="747"/>
+      <c r="N37" s="749"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="781"/>
+      <c r="Q37" s="782"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -64194,11 +64313,11 @@
       <c r="L39" s="61">
         <v>14981.03</v>
       </c>
-      <c r="M39" s="782">
+      <c r="M39" s="783">
         <f>M36+N36</f>
         <v>2934972.49</v>
       </c>
-      <c r="N39" s="783"/>
+      <c r="N39" s="784"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3450079.65</v>
@@ -64446,26 +64565,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="700" t="s">
+      <c r="H52" s="701" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="701"/>
+      <c r="I52" s="702"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="702">
+      <c r="K52" s="703">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="735"/>
+      <c r="L52" s="736"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="706" t="s">
+      <c r="D53" s="707" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="706"/>
+      <c r="E53" s="707"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -64474,22 +64593,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="736" t="s">
+      <c r="D54" s="737" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="736"/>
+      <c r="E54" s="737"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="707" t="s">
+      <c r="I54" s="708" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="708"/>
-      <c r="K54" s="709">
+      <c r="J54" s="709"/>
+      <c r="K54" s="710">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="709"/>
+      <c r="L54" s="710"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -64530,11 +64649,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="711">
+      <c r="K56" s="712">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="712"/>
+      <c r="L56" s="713"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -64551,22 +64670,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="689" t="s">
+      <c r="D58" s="690" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="690"/>
+      <c r="E58" s="691"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="691" t="s">
+      <c r="I58" s="692" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="692"/>
-      <c r="K58" s="693">
+      <c r="J58" s="693"/>
+      <c r="K58" s="694">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="693"/>
+      <c r="L58" s="694"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>

</xml_diff>